<commit_message>
Added decals and todays expenses
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -11,6 +11,8 @@
     <sheet name="Daily Expenses" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Category Analysis" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="M-Pesa Fees" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Outstanding Balances" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Unpaid Labor" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -45,9 +47,17 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="00CC0000"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00E74C3C"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -58,6 +68,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00366092"/>
         <bgColor rgb="00366092"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFCCCC"/>
+        <bgColor rgb="00FFCCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -79,14 +95,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -452,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,7 +520,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KES 199,317</t>
+          <t>KES 229,333</t>
         </is>
       </c>
     </row>
@@ -513,7 +532,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES 800,683</t>
+          <t>KES 770,667</t>
         </is>
       </c>
     </row>
@@ -525,7 +544,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>19.93%</t>
+          <t>22.93%</t>
         </is>
       </c>
     </row>
@@ -537,186 +556,241 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KES 2,357</t>
+          <t>KES 2,693</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
+          <t>Outstanding Amounts</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Outstanding Balances:</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>KES 21,000</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Unpaid Labor:</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>KES 4,300</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Total Pending:</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>KES 25,300</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Effective Balance:</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>KES 745,367</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
           <t>Category Breakdown</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="3" t="inlineStr">
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="B17" s="3" t="inlineStr">
         <is>
           <t>Amount Spent</t>
         </is>
       </c>
-      <c r="C11" s="3" t="inlineStr">
+      <c r="C17" s="3" t="inlineStr">
         <is>
           <t>M-Pesa Fees</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="D17" s="3" t="inlineStr">
         <is>
           <t>Total Cost</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="E17" s="3" t="inlineStr">
         <is>
           <t>Budget %</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Metal &amp; Steel</t>
-        </is>
-      </c>
-      <c r="B12" s="4" t="n">
-        <v>78910</v>
-      </c>
-      <c r="C12" s="4" t="n">
-        <v>1018</v>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>79928</v>
-      </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>7.99%</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="inlineStr">
-        <is>
-          <t>Building Materials</t>
-        </is>
-      </c>
-      <c r="B13" s="4" t="n">
-        <v>77850</v>
-      </c>
-      <c r="C13" s="4" t="n">
-        <v>894</v>
-      </c>
-      <c r="D13" s="4" t="n">
-        <v>78744</v>
-      </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>7.87%</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>Hardware Items</t>
-        </is>
-      </c>
-      <c r="B14" s="4" t="n">
-        <v>15400</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>180</v>
-      </c>
-      <c r="D14" s="4" t="n">
-        <v>15580</v>
-      </c>
-      <c r="E14" s="4" t="inlineStr">
-        <is>
-          <t>1.56%</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="inlineStr">
-        <is>
-          <t>Workers Accommodation</t>
-        </is>
-      </c>
-      <c r="B15" s="4" t="n">
-        <v>13500</v>
-      </c>
-      <c r="C15" s="4" t="n">
-        <v>140</v>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>13640</v>
-      </c>
-      <c r="E15" s="4" t="inlineStr">
-        <is>
-          <t>1.36%</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t>Transport &amp; Logistics</t>
-        </is>
-      </c>
-      <c r="B16" s="4" t="n">
-        <v>7000</v>
-      </c>
-      <c r="C16" s="4" t="n">
-        <v>75</v>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>7075</v>
-      </c>
-      <c r="E16" s="4" t="inlineStr">
-        <is>
-          <t>0.71%</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="inlineStr">
-        <is>
-          <t>Labor Costs</t>
-        </is>
-      </c>
-      <c r="B17" s="4" t="n">
-        <v>3300</v>
-      </c>
-      <c r="C17" s="4" t="n">
-        <v>40</v>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>3340</v>
-      </c>
-      <c r="E17" s="4" t="inlineStr">
-        <is>
-          <t>0.33%</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
         <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>85050</v>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>969</v>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>86019</v>
+      </c>
+      <c r="E18" s="4" t="inlineStr">
+        <is>
+          <t>8.60%</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="inlineStr">
+        <is>
+          <t>Metal &amp; Steel</t>
+        </is>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>78910</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>1018</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>79928</v>
+      </c>
+      <c r="E19" s="4" t="inlineStr">
+        <is>
+          <t>7.99%</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Items</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="n">
+        <v>23180</v>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>23440</v>
+      </c>
+      <c r="E20" s="4" t="inlineStr">
+        <is>
+          <t>2.34%</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="n">
+        <v>15300</v>
+      </c>
+      <c r="C21" s="4" t="n">
+        <v>196</v>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>15496</v>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
+          <t>1.55%</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="inlineStr">
+        <is>
+          <t>Workers Accommodation</t>
+        </is>
+      </c>
+      <c r="B22" s="4" t="n">
+        <v>13500</v>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>140</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>13640</v>
+      </c>
+      <c r="E22" s="4" t="inlineStr">
+        <is>
+          <t>1.36%</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="inlineStr">
+        <is>
+          <t>Transport &amp; Logistics</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="n">
+        <v>9700</v>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>9800</v>
+      </c>
+      <c r="E23" s="4" t="inlineStr">
+        <is>
+          <t>0.98%</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="inlineStr">
+        <is>
           <t>Miscellaneous</t>
         </is>
       </c>
-      <c r="B18" s="4" t="n">
+      <c r="B24" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="C18" s="4" t="n">
+      <c r="C24" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="D18" s="4" t="n">
+      <c r="D24" s="4" t="n">
         <v>1010</v>
       </c>
-      <c r="E18" s="4" t="inlineStr">
+      <c r="E24" s="4" t="inlineStr">
         <is>
           <t>0.10%</t>
         </is>
@@ -736,7 +810,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -752,6 +826,7 @@
     <col width="18" customWidth="1" min="6" max="6"/>
     <col width="18" customWidth="1" min="7" max="7"/>
     <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -795,6 +870,11 @@
           <t>Vendor</t>
         </is>
       </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="inlineStr">
@@ -831,6 +911,11 @@
           <t>Local Transport</t>
         </is>
       </c>
+      <c r="I2" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
@@ -867,6 +952,11 @@
           <t>Transport Company</t>
         </is>
       </c>
+      <c r="I3" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
@@ -903,6 +993,11 @@
           <t>Transport Company</t>
         </is>
       </c>
+      <c r="I4" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
@@ -939,6 +1034,11 @@
           <t>Local Lodge</t>
         </is>
       </c>
+      <c r="I5" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
@@ -975,6 +1075,11 @@
           <t>Property Owner</t>
         </is>
       </c>
+      <c r="I6" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
@@ -1011,6 +1116,11 @@
           <t>Furniture Store</t>
         </is>
       </c>
+      <c r="I7" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
@@ -1047,6 +1157,11 @@
           <t>Sand Supplier</t>
         </is>
       </c>
+      <c r="I8" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
@@ -1083,6 +1198,11 @@
           <t>Ballast Supplier</t>
         </is>
       </c>
+      <c r="I9" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
@@ -1119,6 +1239,11 @@
           <t>Block Manufacturer</t>
         </is>
       </c>
+      <c r="I10" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
@@ -1155,6 +1280,11 @@
           <t>Cement Dealer</t>
         </is>
       </c>
+      <c r="I11" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
@@ -1191,6 +1321,11 @@
           <t>Hardware Store</t>
         </is>
       </c>
+      <c r="I12" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
@@ -1227,6 +1362,11 @@
           <t>Hardware Store</t>
         </is>
       </c>
+      <c r="I13" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
@@ -1263,6 +1403,11 @@
           <t>Hardware Store</t>
         </is>
       </c>
+      <c r="I14" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
@@ -1299,6 +1444,11 @@
           <t>Hardware Store</t>
         </is>
       </c>
+      <c r="I15" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
@@ -1335,6 +1485,11 @@
           <t>Hardware Store</t>
         </is>
       </c>
+      <c r="I16" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
@@ -1371,6 +1526,11 @@
           <t>Hardware Store</t>
         </is>
       </c>
+      <c r="I17" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
@@ -1407,6 +1567,11 @@
           <t>Hardware Store</t>
         </is>
       </c>
+      <c r="I18" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
@@ -1443,6 +1608,11 @@
           <t>Hardware Store</t>
         </is>
       </c>
+      <c r="I19" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
@@ -1479,6 +1649,11 @@
           <t>Hardware Store</t>
         </is>
       </c>
+      <c r="I20" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
@@ -1515,6 +1690,11 @@
           <t>Hardware Store</t>
         </is>
       </c>
+      <c r="I21" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
@@ -1551,6 +1731,11 @@
           <t>Hardware Store</t>
         </is>
       </c>
+      <c r="I22" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
@@ -1587,6 +1772,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I23" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="inlineStr">
@@ -1623,6 +1813,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I24" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="inlineStr">
@@ -1659,6 +1854,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I25" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="inlineStr">
@@ -1695,6 +1895,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I26" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="inlineStr">
@@ -1731,6 +1936,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I27" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="inlineStr">
@@ -1767,6 +1977,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I28" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="inlineStr">
@@ -1803,6 +2018,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I29" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="inlineStr">
@@ -1839,6 +2059,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I30" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
@@ -1875,6 +2100,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I31" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
@@ -1911,6 +2141,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I32" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
@@ -1947,6 +2182,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I33" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="inlineStr">
@@ -1983,6 +2223,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I34" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
@@ -2019,6 +2264,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I35" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="inlineStr">
@@ -2055,6 +2305,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I36" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="4" t="inlineStr">
@@ -2091,6 +2346,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I37" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="inlineStr">
@@ -2127,6 +2387,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I38" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
@@ -2163,6 +2428,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I39" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="inlineStr">
@@ -2199,6 +2469,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I40" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="4" t="inlineStr">
@@ -2235,6 +2510,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I41" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="4" t="inlineStr">
@@ -2271,6 +2551,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I42" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="4" t="inlineStr">
@@ -2307,6 +2592,11 @@
           <t>Metal Supplier</t>
         </is>
       </c>
+      <c r="I43" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="4" t="inlineStr">
@@ -2343,6 +2633,11 @@
           <t>Worker</t>
         </is>
       </c>
+      <c r="I44" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="4" t="inlineStr">
@@ -2379,6 +2674,11 @@
           <t>Worker</t>
         </is>
       </c>
+      <c r="I45" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="4" t="inlineStr">
@@ -2413,6 +2713,462 @@
       <c r="H46" s="4" t="inlineStr">
         <is>
           <t>Unknown</t>
+        </is>
+      </c>
+      <c r="I46" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B47" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C47" s="4" t="inlineStr">
+        <is>
+          <t>Specialist Labor</t>
+        </is>
+      </c>
+      <c r="D47" s="4" t="inlineStr">
+        <is>
+          <t>Welder deposit</t>
+        </is>
+      </c>
+      <c r="E47" s="4" t="n">
+        <v>12000</v>
+      </c>
+      <c r="F47" s="4" t="n">
+        <v>156</v>
+      </c>
+      <c r="G47" s="4" t="n">
+        <v>12156</v>
+      </c>
+      <c r="H47" s="4" t="inlineStr">
+        <is>
+          <t>Welder</t>
+        </is>
+      </c>
+      <c r="I47" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B48" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Items</t>
+        </is>
+      </c>
+      <c r="C48" s="4" t="inlineStr">
+        <is>
+          <t>Tools</t>
+        </is>
+      </c>
+      <c r="D48" s="4" t="inlineStr">
+        <is>
+          <t>Wheelbarrow</t>
+        </is>
+      </c>
+      <c r="E48" s="4" t="n">
+        <v>4350</v>
+      </c>
+      <c r="F48" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="G48" s="4" t="n">
+        <v>4390</v>
+      </c>
+      <c r="H48" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I48" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B49" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Items</t>
+        </is>
+      </c>
+      <c r="C49" s="4" t="inlineStr">
+        <is>
+          <t>Plumbing</t>
+        </is>
+      </c>
+      <c r="D49" s="4" t="inlineStr">
+        <is>
+          <t>Tap 1/2"</t>
+        </is>
+      </c>
+      <c r="E49" s="4" t="n">
+        <v>550</v>
+      </c>
+      <c r="F49" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G49" s="4" t="n">
+        <v>560</v>
+      </c>
+      <c r="H49" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I49" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B50" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Items</t>
+        </is>
+      </c>
+      <c r="C50" s="4" t="inlineStr">
+        <is>
+          <t>Storage</t>
+        </is>
+      </c>
+      <c r="D50" s="4" t="inlineStr">
+        <is>
+          <t>Blue drum</t>
+        </is>
+      </c>
+      <c r="E50" s="4" t="n">
+        <v>2600</v>
+      </c>
+      <c r="F50" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="G50" s="4" t="n">
+        <v>2625</v>
+      </c>
+      <c r="H50" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I50" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B51" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Items</t>
+        </is>
+      </c>
+      <c r="C51" s="4" t="inlineStr">
+        <is>
+          <t>Tools</t>
+        </is>
+      </c>
+      <c r="D51" s="4" t="inlineStr">
+        <is>
+          <t>Hacksaw 14"</t>
+        </is>
+      </c>
+      <c r="E51" s="4" t="n">
+        <v>280</v>
+      </c>
+      <c r="F51" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G51" s="4" t="n">
+        <v>285</v>
+      </c>
+      <c r="H51" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I51" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B52" s="4" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C52" s="4" t="inlineStr">
+        <is>
+          <t>Doors &amp; Windows</t>
+        </is>
+      </c>
+      <c r="D52" s="4" t="inlineStr">
+        <is>
+          <t>Door Frames 6 @ 1200</t>
+        </is>
+      </c>
+      <c r="E52" s="4" t="n">
+        <v>7200</v>
+      </c>
+      <c r="F52" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="G52" s="4" t="n">
+        <v>7275</v>
+      </c>
+      <c r="H52" s="4" t="inlineStr">
+        <is>
+          <t>Carpenter</t>
+        </is>
+      </c>
+      <c r="I52" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B53" s="4" t="inlineStr">
+        <is>
+          <t>Transport &amp; Logistics</t>
+        </is>
+      </c>
+      <c r="C53" s="4" t="inlineStr">
+        <is>
+          <t>Worker Transport</t>
+        </is>
+      </c>
+      <c r="D53" s="4" t="inlineStr">
+        <is>
+          <t>Transport for two electricians to voi</t>
+        </is>
+      </c>
+      <c r="E53" s="4" t="n">
+        <v>2700</v>
+      </c>
+      <c r="F53" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="G53" s="4" t="n">
+        <v>2725</v>
+      </c>
+      <c r="H53" s="4" t="inlineStr">
+        <is>
+          <t>Transport Service</t>
+        </is>
+      </c>
+      <c r="I53" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="5" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B54" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C54" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D54" s="5" t="inlineStr">
+        <is>
+          <t>Jack - Daily Labor (UNPAID)</t>
+        </is>
+      </c>
+      <c r="E54" s="5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F54" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I54" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="5" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B55" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C55" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D55" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - Daily Labor (UNPAID)</t>
+        </is>
+      </c>
+      <c r="E55" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F55" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I55" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="5" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B56" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C56" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D56" s="5" t="inlineStr">
+        <is>
+          <t>Helper 1 - Daily Labor (UNPAID)</t>
+        </is>
+      </c>
+      <c r="E56" s="5" t="n">
+        <v>500</v>
+      </c>
+      <c r="F56" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I56" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="5" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B57" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C57" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D57" s="5" t="inlineStr">
+        <is>
+          <t>Helper 2 - Daily Labor (UNPAID)</t>
+        </is>
+      </c>
+      <c r="E57" s="5" t="n">
+        <v>500</v>
+      </c>
+      <c r="F57" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I57" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
         </is>
       </c>
     </row>
@@ -2461,29 +3217,29 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="inlineStr">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>Fee Structure</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="8" t="inlineStr">
         <is>
           <t>Amount Range</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
+      <c r="B4" s="8" t="inlineStr">
         <is>
           <t>Fee (KES)</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr">
+      <c r="C4" s="8" t="inlineStr">
         <is>
           <t>Transactions</t>
         </is>
       </c>
-      <c r="D4" s="6" t="inlineStr">
+      <c r="D4" s="8" t="inlineStr">
         <is>
           <t>Total Fees</t>
         </is>
@@ -2499,10 +3255,10 @@
         <v>25</v>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>200</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6">
@@ -2515,10 +3271,10 @@
         <v>40</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7">
@@ -2531,10 +3287,10 @@
         <v>75</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>150</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8">
@@ -2595,7 +3351,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" t="n">
         <v>120</v>
@@ -2611,10 +3367,10 @@
         <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13">
@@ -2643,10 +3399,10 @@
         <v>156</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>156</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15">
@@ -2659,10 +3415,10 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D15" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18">
@@ -2671,13 +3427,251 @@
           <t>Total M-Pesa Fees:</t>
         </is>
       </c>
-      <c r="B18" s="5" t="inlineStr">
-        <is>
-          <t>KES 2,357</t>
+      <c r="B18" s="7" t="inlineStr">
+        <is>
+          <t>KES 2,693</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="40" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>OUTSTANDING BALANCES</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Vendor</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>Due Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>Welder</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Remaining balance for welding work</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>21000</v>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>To be scheduled</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>Total Outstanding:</t>
+        </is>
+      </c>
+      <c r="C6" s="7" t="inlineStr">
+        <is>
+          <t>KES 21,000</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>UNPAID LABOR EXPENSES</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Jack - Daily Labor</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D4" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 1 - Daily Labor</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D5" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Helper 1 - Daily Labor</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="D6" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Helper 2 - Daily Labor</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="D7" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>Total Unpaid Labor:</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr">
+        <is>
+          <t>KES 4,300</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Balance reconciliation and transaction fee cleanup - adjusted personal use amount to match actual bank balance of 202,000 KES, removed all transaction fees from Miscellaneous category, updated Excel workbook with synchronized financial data
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KES 749,413</t>
+          <t>KES 798,000</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES 250,587</t>
+          <t>KES 202,000</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>74.94%</t>
+          <t>79.8%</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KES 8,668</t>
+          <t>KES 8,909</t>
         </is>
       </c>
     </row>
@@ -558,7 +558,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>KES 54,400</t>
+          <t>KES 30,000</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KES 54,400</t>
+          <t>KES 30,000</t>
         </is>
       </c>
     </row>
@@ -594,7 +594,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KES 803,813</t>
+          <t>KES 828,000</t>
         </is>
       </c>
     </row>
@@ -606,7 +606,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>80.38%</t>
+          <t>82.80%</t>
         </is>
       </c>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KES 196,187</t>
+          <t>KES 172,000</t>
         </is>
       </c>
     </row>
@@ -659,63 +659,63 @@
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>Labor Costs</t>
+          <t>Building Materials</t>
         </is>
       </c>
       <c r="B20" s="4" t="n">
-        <v>200900</v>
+        <v>183580</v>
       </c>
       <c r="C20" s="4" t="n">
-        <v>2181</v>
+        <v>2300</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>203081</v>
+        <v>185880</v>
       </c>
       <c r="E20" s="4" t="inlineStr">
         <is>
-          <t>20.31%</t>
+          <t>18.59%</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Building Materials</t>
+          <t>Metal &amp; Steel</t>
         </is>
       </c>
       <c r="B21" s="4" t="n">
-        <v>183580</v>
+        <v>176310</v>
       </c>
       <c r="C21" s="4" t="n">
-        <v>2300</v>
+        <v>2090.5</v>
       </c>
       <c r="D21" s="4" t="n">
-        <v>185880</v>
+        <v>178400.5</v>
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>18.59%</t>
+          <t>17.84%</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Metal &amp; Steel</t>
+          <t>Labor Costs</t>
         </is>
       </c>
       <c r="B22" s="4" t="n">
-        <v>176310</v>
+        <v>172700</v>
       </c>
       <c r="C22" s="4" t="n">
-        <v>2090.5</v>
+        <v>1972.5</v>
       </c>
       <c r="D22" s="4" t="n">
-        <v>178400.5</v>
+        <v>174672.5</v>
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>17.84%</t>
+          <t>17.47%</t>
         </is>
       </c>
     </row>
@@ -743,105 +743,105 @@
     <row r="24">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>Workers Accommodation</t>
+          <t>Miscellaneous</t>
         </is>
       </c>
       <c r="B24" s="4" t="n">
-        <v>17760</v>
+        <v>78545.5</v>
       </c>
       <c r="C24" s="4" t="n">
-        <v>190</v>
+        <v>470</v>
       </c>
       <c r="D24" s="4" t="n">
-        <v>17950</v>
+        <v>79015.5</v>
       </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
-          <t>1.80%</t>
+          <t>7.90%</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>Transport &amp; Logistics</t>
+          <t>Workers Accommodation</t>
         </is>
       </c>
       <c r="B25" s="4" t="n">
-        <v>16550</v>
+        <v>17760</v>
       </c>
       <c r="C25" s="4" t="n">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>16735</v>
+        <v>17950</v>
       </c>
       <c r="E25" s="4" t="inlineStr">
         <is>
-          <t>1.67%</t>
+          <t>1.80%</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Transport &amp; Logistics</t>
         </is>
       </c>
       <c r="B26" s="4" t="n">
-        <v>8330</v>
+        <v>16550</v>
       </c>
       <c r="C26" s="4" t="n">
-        <v>85</v>
+        <v>185</v>
       </c>
       <c r="D26" s="4" t="n">
-        <v>8415</v>
+        <v>16735</v>
       </c>
       <c r="E26" s="4" t="inlineStr">
         <is>
-          <t>0.84%</t>
+          <t>1.67%</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="inlineStr">
         <is>
-          <t>Utilities &amp; Services</t>
+          <t>Utilities</t>
         </is>
       </c>
       <c r="B27" s="4" t="n">
-        <v>5100</v>
+        <v>8330</v>
       </c>
       <c r="C27" s="4" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D27" s="4" t="n">
-        <v>5175</v>
+        <v>8415</v>
       </c>
       <c r="E27" s="4" t="inlineStr">
         <is>
-          <t>0.52%</t>
+          <t>0.84%</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="inlineStr">
         <is>
-          <t>Miscellaneous</t>
+          <t>Utilities &amp; Services</t>
         </is>
       </c>
       <c r="B28" s="4" t="n">
-        <v>2000</v>
+        <v>5100</v>
       </c>
       <c r="C28" s="4" t="n">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="D28" s="4" t="n">
-        <v>2020</v>
+        <v>5175</v>
       </c>
       <c r="E28" s="4" t="inlineStr">
         <is>
-          <t>0.20%</t>
+          <t>0.52%</t>
         </is>
       </c>
     </row>
@@ -859,7 +859,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I248"/>
+  <dimension ref="A1:I249"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10978,31 +10978,31 @@
       </c>
       <c r="B247" s="4" t="inlineStr">
         <is>
-          <t>Labor Costs</t>
+          <t>Miscellaneous</t>
         </is>
       </c>
       <c r="C247" s="4" t="inlineStr">
         <is>
-          <t>Labor Payment</t>
+          <t>Not used for the project</t>
         </is>
       </c>
       <c r="D247" s="4" t="inlineStr">
         <is>
-          <t>Payment of all accumulated unpaid labor</t>
+          <t>Money that has been taken out for personal use.</t>
         </is>
       </c>
       <c r="E247" s="4" t="n">
-        <v>52600</v>
+        <v>77045.5</v>
       </c>
       <c r="F247" s="4" t="n">
         <v>455</v>
       </c>
       <c r="G247" s="4" t="n">
-        <v>53055</v>
+        <v>77500.5</v>
       </c>
       <c r="H247" s="4" t="inlineStr">
         <is>
-          <t>Workers</t>
+          <t>Self</t>
         </is>
       </c>
       <c r="I247" s="4" t="inlineStr">
@@ -11014,39 +11014,80 @@
     <row r="248">
       <c r="A248" s="4" t="inlineStr">
         <is>
+          <t>24/09/2025</t>
+        </is>
+      </c>
+      <c r="B248" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C248" s="4" t="inlineStr">
+        <is>
+          <t>Specialized Labor</t>
+        </is>
+      </c>
+      <c r="D248" s="4" t="inlineStr">
+        <is>
+          <t>Welder - final balance payment (18000 of 40000 total)</t>
+        </is>
+      </c>
+      <c r="E248" s="4" t="n">
+        <v>18000</v>
+      </c>
+      <c r="F248" s="4" t="n">
+        <v>171.5</v>
+      </c>
+      <c r="G248" s="4" t="n">
+        <v>18171.5</v>
+      </c>
+      <c r="H248" s="4" t="inlineStr">
+        <is>
+          <t>Welder</t>
+        </is>
+      </c>
+      <c r="I248" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="4" t="inlineStr">
+        <is>
           <t>25/09/2025</t>
         </is>
       </c>
-      <c r="B248" s="4" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="C248" s="4" t="inlineStr">
-        <is>
-          <t>Transaction Fees</t>
-        </is>
-      </c>
-      <c r="D248" s="4" t="inlineStr">
-        <is>
-          <t>M-Pesa processing fees for labor payments</t>
-        </is>
-      </c>
-      <c r="E248" s="4" t="n">
-        <v>500</v>
-      </c>
-      <c r="F248" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="G248" s="4" t="n">
-        <v>505</v>
-      </c>
-      <c r="H248" s="4" t="inlineStr">
-        <is>
-          <t>M-Pesa</t>
-        </is>
-      </c>
-      <c r="I248" s="4" t="inlineStr">
+      <c r="B249" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C249" s="4" t="inlineStr">
+        <is>
+          <t>Specialized Labor</t>
+        </is>
+      </c>
+      <c r="D249" s="4" t="inlineStr">
+        <is>
+          <t>Excavation Worker - final balance payment (6400 of 16000 total)</t>
+        </is>
+      </c>
+      <c r="E249" s="4" t="n">
+        <v>6400</v>
+      </c>
+      <c r="F249" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="G249" s="4" t="n">
+        <v>6475</v>
+      </c>
+      <c r="H249" s="4" t="inlineStr">
+        <is>
+          <t>Excavation Worker</t>
+        </is>
+      </c>
+      <c r="I249" s="4" t="inlineStr">
         <is>
           <t>PAID</t>
         </is>
@@ -11167,10 +11208,10 @@
         <v>75</v>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>750</v>
+        <v>825</v>
       </c>
     </row>
     <row r="8">
@@ -11199,10 +11240,10 @@
         <v>171.5</v>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" t="n">
-        <v>686</v>
+        <v>857.5</v>
       </c>
     </row>
     <row r="10">
@@ -11295,10 +11336,10 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" t="n">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16">
@@ -11341,7 +11382,7 @@
       </c>
       <c r="B20" s="5" t="inlineStr">
         <is>
-          <t>KES 8,668</t>
+          <t>KES 8,909</t>
         </is>
       </c>
     </row>
@@ -11356,7 +11397,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11402,12 +11443,12 @@
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>Welder</t>
+          <t>Electrician</t>
         </is>
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>Remaining balance for welding work (18000 of 40000)</t>
+          <t>Remaining balance for electrical work (18000 of 28000)</t>
         </is>
       </c>
       <c r="C4" s="4" t="n">
@@ -11415,23 +11456,23 @@
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t>24/09/2025</t>
+          <t>To be scheduled</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>Excavation Worker</t>
+          <t>Plumber</t>
         </is>
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>Remaining balance for septic tank digging (6400 of 16000)</t>
+          <t>Remaining balance for plumbing work (12000 of 27000)</t>
         </is>
       </c>
       <c r="C5" s="4" t="n">
-        <v>6400</v>
+        <v>12000</v>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
@@ -11439,55 +11480,15 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Electrician</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Remaining balance for electrical work (18000 of 28000)</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>18000</v>
-      </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>To be scheduled</t>
-        </is>
-      </c>
-    </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>Plumber</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Remaining balance for plumbing work (12000 of 27000)</t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="n">
-        <v>12000</v>
-      </c>
-      <c r="D7" s="4" t="inlineStr">
-        <is>
-          <t>To be scheduled</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="inlineStr">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>Total Outstanding:</t>
         </is>
       </c>
-      <c r="C9" s="5" t="inlineStr">
-        <is>
-          <t>KES 54,400</t>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>KES 30,000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated up to monday
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -47,9 +47,17 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="00CC0000"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00E74C3C"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -60,6 +68,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00366092"/>
         <bgColor rgb="00366092"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFCCCC"/>
+        <bgColor rgb="00FFCCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -81,14 +95,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -503,7 +520,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KES 798,000</t>
+          <t>KES 881,000</t>
         </is>
       </c>
     </row>
@@ -515,7 +532,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES 202,000</t>
+          <t>KES 119,000</t>
         </is>
       </c>
     </row>
@@ -527,7 +544,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>79.8%</t>
+          <t>88.1%</t>
         </is>
       </c>
     </row>
@@ -539,7 +556,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KES 8,909</t>
+          <t>KES 9,913</t>
         </is>
       </c>
     </row>
@@ -570,7 +587,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>KES 0</t>
+          <t>KES 16,200</t>
         </is>
       </c>
     </row>
@@ -582,7 +599,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KES 30,000</t>
+          <t>KES 46,200</t>
         </is>
       </c>
     </row>
@@ -594,7 +611,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KES 828,000</t>
+          <t>KES 927,200</t>
         </is>
       </c>
     </row>
@@ -606,7 +623,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>82.80%</t>
+          <t>92.72%</t>
         </is>
       </c>
     </row>
@@ -618,7 +635,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KES 172,000</t>
+          <t>KES 72,800</t>
         </is>
       </c>
     </row>
@@ -663,59 +680,59 @@
         </is>
       </c>
       <c r="B20" s="4" t="n">
-        <v>183580</v>
+        <v>240370</v>
       </c>
       <c r="C20" s="4" t="n">
-        <v>2300</v>
+        <v>3063</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>185880</v>
+        <v>243433</v>
       </c>
       <c r="E20" s="4" t="inlineStr">
         <is>
-          <t>18.59%</t>
+          <t>24.34%</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>Metal &amp; Steel</t>
+          <t>Labor Costs</t>
         </is>
       </c>
       <c r="B21" s="4" t="n">
-        <v>176310</v>
+        <v>192800</v>
       </c>
       <c r="C21" s="4" t="n">
-        <v>2090.5</v>
+        <v>2177.5</v>
       </c>
       <c r="D21" s="4" t="n">
-        <v>178400.5</v>
+        <v>194977.5</v>
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>17.84%</t>
+          <t>19.50%</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>Labor Costs</t>
+          <t>Metal &amp; Steel</t>
         </is>
       </c>
       <c r="B22" s="4" t="n">
-        <v>172700</v>
+        <v>176310</v>
       </c>
       <c r="C22" s="4" t="n">
-        <v>1972.5</v>
+        <v>2090.5</v>
       </c>
       <c r="D22" s="4" t="n">
-        <v>174672.5</v>
+        <v>178400.5</v>
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>17.47%</t>
+          <t>17.84%</t>
         </is>
       </c>
     </row>
@@ -726,17 +743,17 @@
         </is>
       </c>
       <c r="B23" s="4" t="n">
-        <v>130215</v>
+        <v>130465</v>
       </c>
       <c r="C23" s="4" t="n">
-        <v>1541.5</v>
+        <v>1547.5</v>
       </c>
       <c r="D23" s="4" t="n">
-        <v>131756.5</v>
+        <v>132012.5</v>
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
-          <t>13.18%</t>
+          <t>13.20%</t>
         </is>
       </c>
     </row>
@@ -747,17 +764,17 @@
         </is>
       </c>
       <c r="B24" s="4" t="n">
-        <v>78545.5</v>
+        <v>80901.5</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>470</v>
       </c>
       <c r="D24" s="4" t="n">
-        <v>79015.5</v>
+        <v>81371.5</v>
       </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
-          <t>7.90%</t>
+          <t>8.14%</t>
         </is>
       </c>
     </row>
@@ -768,17 +785,17 @@
         </is>
       </c>
       <c r="B25" s="4" t="n">
-        <v>17760</v>
+        <v>18760</v>
       </c>
       <c r="C25" s="4" t="n">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>17950</v>
+        <v>18960</v>
       </c>
       <c r="E25" s="4" t="inlineStr">
         <is>
-          <t>1.80%</t>
+          <t>1.90%</t>
         </is>
       </c>
     </row>
@@ -789,17 +806,17 @@
         </is>
       </c>
       <c r="B26" s="4" t="n">
-        <v>16550</v>
+        <v>16850</v>
       </c>
       <c r="C26" s="4" t="n">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D26" s="4" t="n">
-        <v>16735</v>
+        <v>17040</v>
       </c>
       <c r="E26" s="4" t="inlineStr">
         <is>
-          <t>1.67%</t>
+          <t>1.70%</t>
         </is>
       </c>
     </row>
@@ -810,17 +827,17 @@
         </is>
       </c>
       <c r="B27" s="4" t="n">
-        <v>8330</v>
+        <v>9530</v>
       </c>
       <c r="C27" s="4" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="D27" s="4" t="n">
-        <v>8415</v>
+        <v>9630</v>
       </c>
       <c r="E27" s="4" t="inlineStr">
         <is>
-          <t>0.84%</t>
+          <t>0.96%</t>
         </is>
       </c>
     </row>
@@ -859,7 +876,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I249"/>
+  <dimension ref="A1:I280"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10988,17 +11005,17 @@
       </c>
       <c r="D247" s="4" t="inlineStr">
         <is>
-          <t>Money that has been taken out for personal use.</t>
+          <t>Money taken for personal use and potential overcharges or unaccounted expenses.</t>
         </is>
       </c>
       <c r="E247" s="4" t="n">
-        <v>77045.5</v>
+        <v>79401.5</v>
       </c>
       <c r="F247" s="4" t="n">
         <v>455</v>
       </c>
       <c r="G247" s="4" t="n">
-        <v>77500.5</v>
+        <v>79856.5</v>
       </c>
       <c r="H247" s="4" t="inlineStr">
         <is>
@@ -11088,6 +11105,1277 @@
         </is>
       </c>
       <c r="I249" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="4" t="inlineStr">
+        <is>
+          <t>26/09/2025</t>
+        </is>
+      </c>
+      <c r="B250" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C250" s="4" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D250" s="4" t="inlineStr">
+        <is>
+          <t>3 Fundi @ 1300 each</t>
+        </is>
+      </c>
+      <c r="E250" s="4" t="n">
+        <v>3900</v>
+      </c>
+      <c r="F250" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="G250" s="4" t="n">
+        <v>3940</v>
+      </c>
+      <c r="H250" s="4" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I250" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="4" t="inlineStr">
+        <is>
+          <t>26/09/2025</t>
+        </is>
+      </c>
+      <c r="B251" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C251" s="4" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D251" s="4" t="inlineStr">
+        <is>
+          <t>2 Fundi @ 1200 each</t>
+        </is>
+      </c>
+      <c r="E251" s="4" t="n">
+        <v>2400</v>
+      </c>
+      <c r="F251" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="G251" s="4" t="n">
+        <v>2425</v>
+      </c>
+      <c r="H251" s="4" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I251" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="4" t="inlineStr">
+        <is>
+          <t>26/09/2025</t>
+        </is>
+      </c>
+      <c r="B252" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C252" s="4" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D252" s="4" t="inlineStr">
+        <is>
+          <t>5 helpers @ 600 each</t>
+        </is>
+      </c>
+      <c r="E252" s="4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F252" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="G252" s="4" t="n">
+        <v>3025</v>
+      </c>
+      <c r="H252" s="4" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I252" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="4" t="inlineStr">
+        <is>
+          <t>26/09/2025</t>
+        </is>
+      </c>
+      <c r="B253" s="4" t="inlineStr">
+        <is>
+          <t>Transport &amp; Logistics</t>
+        </is>
+      </c>
+      <c r="C253" s="4" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="D253" s="4" t="inlineStr">
+        <is>
+          <t>Transport on boda</t>
+        </is>
+      </c>
+      <c r="E253" s="4" t="n">
+        <v>300</v>
+      </c>
+      <c r="F253" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G253" s="4" t="n">
+        <v>305</v>
+      </c>
+      <c r="H253" s="4" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="I253" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="4" t="inlineStr">
+        <is>
+          <t>26/09/2025</t>
+        </is>
+      </c>
+      <c r="B254" s="4" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C254" s="4" t="inlineStr">
+        <is>
+          <t>Sand</t>
+        </is>
+      </c>
+      <c r="D254" s="4" t="inlineStr">
+        <is>
+          <t>Sand 14 tonnes</t>
+        </is>
+      </c>
+      <c r="E254" s="4" t="n">
+        <v>9000</v>
+      </c>
+      <c r="F254" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="G254" s="4" t="n">
+        <v>9096</v>
+      </c>
+      <c r="H254" s="4" t="inlineStr">
+        <is>
+          <t>Supplier</t>
+        </is>
+      </c>
+      <c r="I254" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="4" t="inlineStr">
+        <is>
+          <t>26/09/2025</t>
+        </is>
+      </c>
+      <c r="B255" s="4" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="C255" s="4" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="D255" s="4" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="E255" s="4" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F255" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G255" s="4" t="n">
+        <v>1215</v>
+      </c>
+      <c r="H255" s="4" t="inlineStr">
+        <is>
+          <t>Supplier</t>
+        </is>
+      </c>
+      <c r="I255" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="4" t="inlineStr">
+        <is>
+          <t>26/09/2025</t>
+        </is>
+      </c>
+      <c r="B256" s="4" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C256" s="4" t="inlineStr">
+        <is>
+          <t>Cement</t>
+        </is>
+      </c>
+      <c r="D256" s="4" t="inlineStr">
+        <is>
+          <t>20 bags cement @ 720 each</t>
+        </is>
+      </c>
+      <c r="E256" s="4" t="n">
+        <v>14400</v>
+      </c>
+      <c r="F256" s="4" t="n">
+        <v>156</v>
+      </c>
+      <c r="G256" s="4" t="n">
+        <v>14556</v>
+      </c>
+      <c r="H256" s="4" t="inlineStr">
+        <is>
+          <t>Supplier</t>
+        </is>
+      </c>
+      <c r="I256" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="4" t="inlineStr">
+        <is>
+          <t>26/09/2025</t>
+        </is>
+      </c>
+      <c r="B257" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Items</t>
+        </is>
+      </c>
+      <c r="C257" s="4" t="inlineStr">
+        <is>
+          <t>Plumbing</t>
+        </is>
+      </c>
+      <c r="D257" s="4" t="inlineStr">
+        <is>
+          <t>1 pc G.I union 3/4 @ 130</t>
+        </is>
+      </c>
+      <c r="E257" s="4" t="n">
+        <v>130</v>
+      </c>
+      <c r="F257" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G257" s="4" t="n">
+        <v>135</v>
+      </c>
+      <c r="H257" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I257" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="4" t="inlineStr">
+        <is>
+          <t>26/09/2025</t>
+        </is>
+      </c>
+      <c r="B258" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Items</t>
+        </is>
+      </c>
+      <c r="C258" s="4" t="inlineStr">
+        <is>
+          <t>Plumbing</t>
+        </is>
+      </c>
+      <c r="D258" s="4" t="inlineStr">
+        <is>
+          <t>1 pc G.I R/Socket 3/4 x 1/2 @ 80</t>
+        </is>
+      </c>
+      <c r="E258" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="F258" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G258" s="4" t="n">
+        <v>81</v>
+      </c>
+      <c r="H258" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I258" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="4" t="inlineStr">
+        <is>
+          <t>26/09/2025</t>
+        </is>
+      </c>
+      <c r="B259" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Items</t>
+        </is>
+      </c>
+      <c r="C259" s="4" t="inlineStr">
+        <is>
+          <t>Plumbing</t>
+        </is>
+      </c>
+      <c r="D259" s="4" t="inlineStr">
+        <is>
+          <t>1 pc G.I play 1/2 @ 40</t>
+        </is>
+      </c>
+      <c r="E259" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="F259" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G259" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="H259" s="4" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I259" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="4" t="inlineStr">
+        <is>
+          <t>27/09/2025</t>
+        </is>
+      </c>
+      <c r="B260" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C260" s="4" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D260" s="4" t="inlineStr">
+        <is>
+          <t>Jack</t>
+        </is>
+      </c>
+      <c r="E260" s="4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F260" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G260" s="4" t="n">
+        <v>1515</v>
+      </c>
+      <c r="H260" s="4" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I260" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="4" t="inlineStr">
+        <is>
+          <t>27/09/2025</t>
+        </is>
+      </c>
+      <c r="B261" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C261" s="4" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D261" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 1</t>
+        </is>
+      </c>
+      <c r="E261" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F261" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G261" s="4" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H261" s="4" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I261" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="4" t="inlineStr">
+        <is>
+          <t>27/09/2025</t>
+        </is>
+      </c>
+      <c r="B262" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C262" s="4" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D262" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 2</t>
+        </is>
+      </c>
+      <c r="E262" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F262" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G262" s="4" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H262" s="4" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I262" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="4" t="inlineStr">
+        <is>
+          <t>27/09/2025</t>
+        </is>
+      </c>
+      <c r="B263" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C263" s="4" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D263" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 3</t>
+        </is>
+      </c>
+      <c r="E263" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F263" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G263" s="4" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H263" s="4" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I263" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="4" t="inlineStr">
+        <is>
+          <t>27/09/2025</t>
+        </is>
+      </c>
+      <c r="B264" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C264" s="4" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D264" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 4</t>
+        </is>
+      </c>
+      <c r="E264" s="4" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F264" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G264" s="4" t="n">
+        <v>1215</v>
+      </c>
+      <c r="H264" s="4" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I264" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="4" t="inlineStr">
+        <is>
+          <t>27/09/2025</t>
+        </is>
+      </c>
+      <c r="B265" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C265" s="4" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D265" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 5</t>
+        </is>
+      </c>
+      <c r="E265" s="4" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F265" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G265" s="4" t="n">
+        <v>1215</v>
+      </c>
+      <c r="H265" s="4" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I265" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="4" t="inlineStr">
+        <is>
+          <t>27/09/2025</t>
+        </is>
+      </c>
+      <c r="B266" s="4" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C266" s="4" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D266" s="4" t="inlineStr">
+        <is>
+          <t>5 helpers @ 600 each</t>
+        </is>
+      </c>
+      <c r="E266" s="4" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F266" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="G266" s="4" t="n">
+        <v>3025</v>
+      </c>
+      <c r="H266" s="4" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I266" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="4" t="inlineStr">
+        <is>
+          <t>27/09/2025</t>
+        </is>
+      </c>
+      <c r="B267" s="4" t="inlineStr">
+        <is>
+          <t>Workers Accommodation</t>
+        </is>
+      </c>
+      <c r="C267" s="4" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="D267" s="4" t="inlineStr">
+        <is>
+          <t>Meat for workers</t>
+        </is>
+      </c>
+      <c r="E267" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F267" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G267" s="4" t="n">
+        <v>1010</v>
+      </c>
+      <c r="H267" s="4" t="inlineStr">
+        <is>
+          <t>Supplier</t>
+        </is>
+      </c>
+      <c r="I267" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="5" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="B268" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C268" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D268" s="5" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="E268" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F268" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G268" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H268" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I268" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="5" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="B269" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C269" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D269" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E269" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F269" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G269" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H269" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I269" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="5" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="B270" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C270" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D270" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E270" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F270" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G270" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H270" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I270" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="5" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="B271" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C271" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D271" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E271" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F271" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G271" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H271" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I271" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="5" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="B272" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C272" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D272" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 4 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E272" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F272" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G272" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H272" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I272" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="5" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="B273" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C273" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D273" s="5" t="inlineStr">
+        <is>
+          <t>4 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="E273" s="5" t="n">
+        <v>2400</v>
+      </c>
+      <c r="F273" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G273" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H273" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I273" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="5" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="B274" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C274" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D274" s="5" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="E274" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F274" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G274" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H274" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I274" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="5" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="B275" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C275" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D275" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E275" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F275" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G275" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H275" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I275" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="5" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="B276" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C276" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D276" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E276" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F276" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G276" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H276" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I276" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="5" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="B277" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C277" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D277" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E277" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F277" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G277" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H277" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I277" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="5" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="B278" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C278" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D278" s="5" t="inlineStr">
+        <is>
+          <t>3 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="E278" s="5" t="n">
+        <v>1800</v>
+      </c>
+      <c r="F278" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G278" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H278" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I278" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="4" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="B279" s="4" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C279" s="4" t="inlineStr">
+        <is>
+          <t>Cement</t>
+        </is>
+      </c>
+      <c r="D279" s="4" t="inlineStr">
+        <is>
+          <t>30 bags cement @ 720 each</t>
+        </is>
+      </c>
+      <c r="E279" s="4" t="n">
+        <v>21600</v>
+      </c>
+      <c r="F279" s="4" t="n">
+        <v>355</v>
+      </c>
+      <c r="G279" s="4" t="n">
+        <v>21955</v>
+      </c>
+      <c r="H279" s="4" t="inlineStr">
+        <is>
+          <t>Supplier</t>
+        </is>
+      </c>
+      <c r="I279" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="4" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="B280" s="4" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C280" s="4" t="inlineStr">
+        <is>
+          <t>Stones</t>
+        </is>
+      </c>
+      <c r="D280" s="4" t="inlineStr">
+        <is>
+          <t>262ft 6X9 stones @ 42 sh per ft</t>
+        </is>
+      </c>
+      <c r="E280" s="4" t="n">
+        <v>11790</v>
+      </c>
+      <c r="F280" s="4" t="n">
+        <v>156</v>
+      </c>
+      <c r="G280" s="4" t="n">
+        <v>11946</v>
+      </c>
+      <c r="H280" s="4" t="inlineStr">
+        <is>
+          <t>Supplier</t>
+        </is>
+      </c>
+      <c r="I280" s="4" t="inlineStr">
         <is>
           <t>PAID</t>
         </is>
@@ -11138,29 +12426,29 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="inlineStr">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>Fee Structure</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="8" t="inlineStr">
         <is>
           <t>Amount Range</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
+      <c r="B4" s="8" t="inlineStr">
         <is>
           <t>Fee (KES)</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr">
+      <c r="C4" s="8" t="inlineStr">
         <is>
           <t>Transactions</t>
         </is>
       </c>
-      <c r="D4" s="6" t="inlineStr">
+      <c r="D4" s="8" t="inlineStr">
         <is>
           <t>Total Fees</t>
         </is>
@@ -11176,10 +12464,10 @@
         <v>25</v>
       </c>
       <c r="C5" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D5" t="n">
-        <v>650</v>
+        <v>725</v>
       </c>
     </row>
     <row r="6">
@@ -11192,10 +12480,10 @@
         <v>40</v>
       </c>
       <c r="C6" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" t="n">
-        <v>760</v>
+        <v>800</v>
       </c>
     </row>
     <row r="7">
@@ -11224,10 +12512,10 @@
         <v>96</v>
       </c>
       <c r="C8" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>864</v>
+        <v>960</v>
       </c>
     </row>
     <row r="9">
@@ -11272,10 +12560,10 @@
         <v>15</v>
       </c>
       <c r="C11" t="n">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D11" t="n">
-        <v>735</v>
+        <v>840</v>
       </c>
     </row>
     <row r="12">
@@ -11288,10 +12576,10 @@
         <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D12" t="n">
-        <v>690</v>
+        <v>700</v>
       </c>
     </row>
     <row r="13">
@@ -11304,10 +12592,10 @@
         <v>355</v>
       </c>
       <c r="C13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" t="n">
-        <v>1775</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="14">
@@ -11320,10 +12608,10 @@
         <v>156</v>
       </c>
       <c r="C14" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D14" t="n">
-        <v>624</v>
+        <v>936</v>
       </c>
     </row>
     <row r="15">
@@ -11336,10 +12624,10 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D15" t="n">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16">
@@ -11352,10 +12640,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -11368,7 +12656,7 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -11380,9 +12668,9 @@
           <t>Total M-Pesa Fees:</t>
         </is>
       </c>
-      <c r="B20" s="5" t="inlineStr">
-        <is>
-          <t>KES 8,909</t>
+      <c r="B20" s="7" t="inlineStr">
+        <is>
+          <t>KES 9,913</t>
         </is>
       </c>
     </row>
@@ -11481,12 +12769,12 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="inlineStr">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>Total Outstanding:</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
+      <c r="C7" s="7" t="inlineStr">
         <is>
           <t>KES 30,000</t>
         </is>
@@ -11506,7 +12794,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11549,15 +12837,235 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D4" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
     <row r="5">
-      <c r="A5" s="5" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D5" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D6" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D7" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 4 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D8" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>4 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>2400</v>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D10" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D11" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D12" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D13" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>3 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D14" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
         <is>
           <t>Total Unpaid Labor:</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>KES 0</t>
+      <c r="C16" s="7" t="inlineStr">
+        <is>
+          <t>KES 16,200</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update budget to 1,300,000 KES and regenerate Excel report
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -508,7 +508,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>KES 1,000,000</t>
+          <t>KES 1,300,000</t>
         </is>
       </c>
     </row>
@@ -532,7 +532,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES 119,000</t>
+          <t>KES 419,000</t>
         </is>
       </c>
     </row>
@@ -544,7 +544,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>88.1%</t>
+          <t>67.77%</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>KES 16,200</t>
+          <t>KES 47,300</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KES 46,200</t>
+          <t>KES 77,300</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KES 927,200</t>
+          <t>KES 958,300</t>
         </is>
       </c>
     </row>
@@ -623,7 +623,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>92.72%</t>
+          <t>73.72%</t>
         </is>
       </c>
     </row>
@@ -635,7 +635,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KES 72,800</t>
+          <t>KES 341,700</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="E20" s="4" t="inlineStr">
         <is>
-          <t>24.34%</t>
+          <t>18.73%</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>19.50%</t>
+          <t>15.00%</t>
         </is>
       </c>
     </row>
@@ -732,7 +732,7 @@
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>17.84%</t>
+          <t>13.72%</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
-          <t>13.20%</t>
+          <t>10.15%</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
-          <t>8.14%</t>
+          <t>6.26%</t>
         </is>
       </c>
     </row>
@@ -795,7 +795,7 @@
       </c>
       <c r="E25" s="4" t="inlineStr">
         <is>
-          <t>1.90%</t>
+          <t>1.46%</t>
         </is>
       </c>
     </row>
@@ -816,7 +816,7 @@
       </c>
       <c r="E26" s="4" t="inlineStr">
         <is>
-          <t>1.70%</t>
+          <t>1.31%</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="E27" s="4" t="inlineStr">
         <is>
-          <t>0.96%</t>
+          <t>0.74%</t>
         </is>
       </c>
     </row>
@@ -858,7 +858,7 @@
       </c>
       <c r="E28" s="4" t="inlineStr">
         <is>
-          <t>0.52%</t>
+          <t>0.40%</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I280"/>
+  <dimension ref="A1:I301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12378,6 +12378,867 @@
       <c r="I280" s="4" t="inlineStr">
         <is>
           <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="5" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="B281" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C281" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D281" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E281" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F281" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G281" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H281" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I281" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="5" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="B282" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C282" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D282" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E282" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F282" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G282" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H282" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I282" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="5" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="B283" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C283" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D283" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E283" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F283" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G283" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H283" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I283" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="5" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="B284" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C284" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D284" s="5" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="E284" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F284" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G284" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H284" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I284" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="5" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="B285" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C285" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D285" s="5" t="inlineStr">
+        <is>
+          <t>3 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="E285" s="5" t="n">
+        <v>1800</v>
+      </c>
+      <c r="F285" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G285" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H285" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I285" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="5" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="B286" s="5" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="C286" s="5" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="D286" s="5" t="inlineStr">
+        <is>
+          <t>Water - UNPAID</t>
+        </is>
+      </c>
+      <c r="E286" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F286" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G286" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H286" s="5" t="inlineStr">
+        <is>
+          <t>Supplier</t>
+        </is>
+      </c>
+      <c r="I286" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="5" t="inlineStr">
+        <is>
+          <t>01/10/2025</t>
+        </is>
+      </c>
+      <c r="B287" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C287" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D287" s="5" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="E287" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F287" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G287" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H287" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I287" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="5" t="inlineStr">
+        <is>
+          <t>01/10/2025</t>
+        </is>
+      </c>
+      <c r="B288" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C288" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D288" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E288" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F288" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G288" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H288" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I288" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="5" t="inlineStr">
+        <is>
+          <t>01/10/2025</t>
+        </is>
+      </c>
+      <c r="B289" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C289" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D289" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E289" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F289" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G289" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H289" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I289" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="5" t="inlineStr">
+        <is>
+          <t>01/10/2025</t>
+        </is>
+      </c>
+      <c r="B290" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C290" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D290" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E290" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F290" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G290" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H290" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I290" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="5" t="inlineStr">
+        <is>
+          <t>01/10/2025</t>
+        </is>
+      </c>
+      <c r="B291" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C291" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D291" s="5" t="inlineStr">
+        <is>
+          <t>3 helpers @ 800 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="E291" s="5" t="n">
+        <v>2400</v>
+      </c>
+      <c r="F291" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G291" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H291" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I291" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="5" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="B292" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C292" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D292" s="5" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="E292" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F292" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G292" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H292" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I292" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="5" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="B293" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C293" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D293" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E293" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F293" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G293" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H293" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I293" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="5" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="B294" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C294" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D294" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E294" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F294" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G294" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H294" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I294" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="5" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="B295" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C295" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D295" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E295" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F295" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G295" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H295" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I295" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="5" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="B296" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C296" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D296" s="5" t="inlineStr">
+        <is>
+          <t>3 helpers @ 800 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="E296" s="5" t="n">
+        <v>2400</v>
+      </c>
+      <c r="F296" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G296" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H296" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I296" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="5" t="inlineStr">
+        <is>
+          <t>03/10/2025</t>
+        </is>
+      </c>
+      <c r="B297" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C297" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D297" s="5" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="E297" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F297" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G297" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H297" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I297" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="5" t="inlineStr">
+        <is>
+          <t>03/10/2025</t>
+        </is>
+      </c>
+      <c r="B298" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C298" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D298" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E298" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F298" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G298" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H298" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I298" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="5" t="inlineStr">
+        <is>
+          <t>03/10/2025</t>
+        </is>
+      </c>
+      <c r="B299" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C299" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D299" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E299" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F299" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G299" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H299" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I299" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="5" t="inlineStr">
+        <is>
+          <t>03/10/2025</t>
+        </is>
+      </c>
+      <c r="B300" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C300" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D300" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E300" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F300" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G300" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H300" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I300" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="5" t="inlineStr">
+        <is>
+          <t>03/10/2025</t>
+        </is>
+      </c>
+      <c r="B301" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C301" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D301" s="5" t="inlineStr">
+        <is>
+          <t>3 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="E301" s="5" t="n">
+        <v>1800</v>
+      </c>
+      <c r="F301" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G301" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H301" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I301" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
         </is>
       </c>
     </row>
@@ -12464,7 +13325,7 @@
         <v>25</v>
       </c>
       <c r="C5" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D5" t="n">
         <v>725</v>
@@ -12560,7 +13421,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="n">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D11" t="n">
         <v>840</v>
@@ -12794,7 +13655,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13057,15 +13918,435 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D15" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
     <row r="16">
-      <c r="A16" s="7" t="inlineStr">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D16" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D17" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D18" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>3 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D19" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>Water - UNPAID</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D20" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t>01/10/2025</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="C21" s="4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D21" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="inlineStr">
+        <is>
+          <t>01/10/2025</t>
+        </is>
+      </c>
+      <c r="B22" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D22" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="inlineStr">
+        <is>
+          <t>01/10/2025</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D23" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="inlineStr">
+        <is>
+          <t>01/10/2025</t>
+        </is>
+      </c>
+      <c r="B24" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C24" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D24" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="inlineStr">
+        <is>
+          <t>01/10/2025</t>
+        </is>
+      </c>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>3 helpers @ 800 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="C25" s="4" t="n">
+        <v>2400</v>
+      </c>
+      <c r="D25" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="C26" s="4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D26" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C27" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D27" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="B28" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C28" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D28" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="B29" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C29" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D29" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="B30" s="4" t="inlineStr">
+        <is>
+          <t>3 helpers @ 800 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="C30" s="4" t="n">
+        <v>2400</v>
+      </c>
+      <c r="D30" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="inlineStr">
+        <is>
+          <t>03/10/2025</t>
+        </is>
+      </c>
+      <c r="B31" s="4" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="C31" s="4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D31" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="inlineStr">
+        <is>
+          <t>03/10/2025</t>
+        </is>
+      </c>
+      <c r="B32" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C32" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D32" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="inlineStr">
+        <is>
+          <t>03/10/2025</t>
+        </is>
+      </c>
+      <c r="B33" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C33" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D33" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="inlineStr">
+        <is>
+          <t>03/10/2025</t>
+        </is>
+      </c>
+      <c r="B34" s="4" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C34" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D34" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="inlineStr">
+        <is>
+          <t>03/10/2025</t>
+        </is>
+      </c>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
+          <t>3 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="C35" s="4" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D35" s="9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="7" t="inlineStr">
         <is>
           <t>Total Unpaid Labor:</t>
         </is>
       </c>
-      <c r="C16" s="7" t="inlineStr">
-        <is>
-          <t>KES 16,200</t>
+      <c r="C37" s="7" t="inlineStr">
+        <is>
+          <t>KES 47,300</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Regenerate Excel report with corrected amounts and food supplies
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -520,7 +520,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KES 881,000</t>
+          <t>KES 886,450</t>
         </is>
       </c>
     </row>
@@ -532,7 +532,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES 419,000</t>
+          <t>KES 413,550</t>
         </is>
       </c>
     </row>
@@ -544,7 +544,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>67.77%</t>
+          <t>68.19%</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KES 9,913</t>
+          <t>KES 9,963</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>KES 47,300</t>
+          <t>KES 46,100</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KES 77,300</t>
+          <t>KES 76,100</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KES 958,300</t>
+          <t>KES 962,550</t>
         </is>
       </c>
     </row>
@@ -623,7 +623,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>73.72%</t>
+          <t>74.04%</t>
         </is>
       </c>
     </row>
@@ -635,7 +635,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KES 341,700</t>
+          <t>KES 337,450</t>
         </is>
       </c>
     </row>
@@ -785,17 +785,17 @@
         </is>
       </c>
       <c r="B25" s="4" t="n">
-        <v>18760</v>
+        <v>24160</v>
       </c>
       <c r="C25" s="4" t="n">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>18960</v>
+        <v>24410</v>
       </c>
       <c r="E25" s="4" t="inlineStr">
         <is>
-          <t>1.46%</t>
+          <t>1.88%</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I301"/>
+  <dimension ref="A1:I303"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12809,11 +12809,11 @@
       </c>
       <c r="D291" s="5" t="inlineStr">
         <is>
-          <t>3 helpers @ 800 each - UNPAID</t>
+          <t>3 helpers @ 600 each - UNPAID</t>
         </is>
       </c>
       <c r="E291" s="5" t="n">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="F291" s="5" t="n">
         <v>0</v>
@@ -13014,11 +13014,11 @@
       </c>
       <c r="D296" s="5" t="inlineStr">
         <is>
-          <t>3 helpers @ 800 each - UNPAID</t>
+          <t>3 helpers @ 600 each - UNPAID</t>
         </is>
       </c>
       <c r="E296" s="5" t="n">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="F296" s="5" t="n">
         <v>0</v>
@@ -13038,84 +13038,84 @@
       </c>
     </row>
     <row r="297">
-      <c r="A297" s="5" t="inlineStr">
-        <is>
-          <t>03/10/2025</t>
-        </is>
-      </c>
-      <c r="B297" s="5" t="inlineStr">
-        <is>
-          <t>Labor Costs</t>
-        </is>
-      </c>
-      <c r="C297" s="5" t="inlineStr">
-        <is>
-          <t>Daily Labor</t>
-        </is>
-      </c>
-      <c r="D297" s="5" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="E297" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="F297" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G297" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H297" s="5" t="inlineStr">
-        <is>
-          <t>Worker</t>
-        </is>
-      </c>
-      <c r="I297" s="6" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="A297" s="4" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="B297" s="4" t="inlineStr">
+        <is>
+          <t>Workers Accommodation</t>
+        </is>
+      </c>
+      <c r="C297" s="4" t="inlineStr">
+        <is>
+          <t>Food Supplies</t>
+        </is>
+      </c>
+      <c r="D297" s="4" t="inlineStr">
+        <is>
+          <t>Unga and cooking oil for workers</t>
+        </is>
+      </c>
+      <c r="E297" s="4" t="n">
+        <v>2700</v>
+      </c>
+      <c r="F297" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="G297" s="4" t="n">
+        <v>2725</v>
+      </c>
+      <c r="H297" s="4" t="inlineStr">
+        <is>
+          <t>Supplier</t>
+        </is>
+      </c>
+      <c r="I297" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="298">
-      <c r="A298" s="5" t="inlineStr">
-        <is>
-          <t>03/10/2025</t>
-        </is>
-      </c>
-      <c r="B298" s="5" t="inlineStr">
-        <is>
-          <t>Labor Costs</t>
-        </is>
-      </c>
-      <c r="C298" s="5" t="inlineStr">
-        <is>
-          <t>Daily Labor</t>
-        </is>
-      </c>
-      <c r="D298" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E298" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="F298" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G298" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H298" s="5" t="inlineStr">
-        <is>
-          <t>Worker</t>
-        </is>
-      </c>
-      <c r="I298" s="6" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="A298" s="4" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="B298" s="4" t="inlineStr">
+        <is>
+          <t>Workers Accommodation</t>
+        </is>
+      </c>
+      <c r="C298" s="4" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="D298" s="4" t="inlineStr">
+        <is>
+          <t>Unga and cooking oil for workers</t>
+        </is>
+      </c>
+      <c r="E298" s="4" t="n">
+        <v>2700</v>
+      </c>
+      <c r="F298" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="G298" s="4" t="n">
+        <v>2725</v>
+      </c>
+      <c r="H298" s="4" t="inlineStr">
+        <is>
+          <t>Supplier</t>
+        </is>
+      </c>
+      <c r="I298" s="4" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
@@ -13137,11 +13137,11 @@
       </c>
       <c r="D299" s="5" t="inlineStr">
         <is>
-          <t>Fundi 2 - UNPAID</t>
+          <t>Jack - UNPAID</t>
         </is>
       </c>
       <c r="E299" s="5" t="n">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="F299" s="5" t="n">
         <v>0</v>
@@ -13178,7 +13178,7 @@
       </c>
       <c r="D300" s="5" t="inlineStr">
         <is>
-          <t>Fundi 3 - UNPAID</t>
+          <t>Fundi 1 - UNPAID</t>
         </is>
       </c>
       <c r="E300" s="5" t="n">
@@ -13219,11 +13219,11 @@
       </c>
       <c r="D301" s="5" t="inlineStr">
         <is>
-          <t>3 helpers @ 600 each - UNPAID</t>
+          <t>Fundi 2 - UNPAID</t>
         </is>
       </c>
       <c r="E301" s="5" t="n">
-        <v>1800</v>
+        <v>1300</v>
       </c>
       <c r="F301" s="5" t="n">
         <v>0</v>
@@ -13237,6 +13237,88 @@
         </is>
       </c>
       <c r="I301" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="5" t="inlineStr">
+        <is>
+          <t>03/10/2025</t>
+        </is>
+      </c>
+      <c r="B302" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C302" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D302" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 3 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E302" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F302" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G302" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H302" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I302" s="6" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="5" t="inlineStr">
+        <is>
+          <t>03/10/2025</t>
+        </is>
+      </c>
+      <c r="B303" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C303" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D303" s="5" t="inlineStr">
+        <is>
+          <t>3 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="E303" s="5" t="n">
+        <v>1800</v>
+      </c>
+      <c r="F303" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G303" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H303" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I303" s="6" t="inlineStr">
         <is>
           <t>UNPAID</t>
         </is>
@@ -13325,10 +13407,10 @@
         <v>25</v>
       </c>
       <c r="C5" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D5" t="n">
-        <v>725</v>
+        <v>775</v>
       </c>
     </row>
     <row r="6">
@@ -13531,7 +13613,7 @@
       </c>
       <c r="B20" s="7" t="inlineStr">
         <is>
-          <t>KES 9,913</t>
+          <t>KES 9,963</t>
         </is>
       </c>
     </row>
@@ -14126,11 +14208,11 @@
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>3 helpers @ 800 each - UNPAID</t>
+          <t>3 helpers @ 600 each - UNPAID</t>
         </is>
       </c>
       <c r="C25" s="4" t="n">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="D25" s="9" t="inlineStr">
         <is>
@@ -14226,11 +14308,11 @@
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>3 helpers @ 800 each - UNPAID</t>
+          <t>3 helpers @ 600 each - UNPAID</t>
         </is>
       </c>
       <c r="C30" s="4" t="n">
-        <v>2400</v>
+        <v>1800</v>
       </c>
       <c r="D30" s="9" t="inlineStr">
         <is>
@@ -14346,7 +14428,7 @@
       </c>
       <c r="C37" s="7" t="inlineStr">
         <is>
-          <t>KES 47,300</t>
+          <t>KES 46,100</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Oct 21 labor and materials entries
- Labor (5,300 UNPAID): Jack 1,500, Fundi 1 & 2 @ 1,300 each, 2 helpers @ 600 each
- Materials (10,230 PAID): 17ft faceboard 1,530, 6 ceiling board 6,300, aluminium corners 2,000, spacers 400
- Total spent: 1,473,573.5 (147.36% of budget)
- Unpaid labor now: 15,900
- Total pending: 292,905
- Additional funds needed: 766,478.5 (76.65% over budget)
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -540,7 +540,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>KES 1,490,000</t>
+          <t>KES 1,000,000</t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KES 1,463,213</t>
+          <t>KES 1,473,573</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES 26,786</t>
+          <t>KES -473,573</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>98.2%</t>
+          <t>147.36%</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KES 16,771</t>
+          <t>KES 16,901</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>KES 10,600</t>
+          <t>KES 15,900</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KES 101,900</t>
+          <t>KES 107,200</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KES 1,565,113</t>
+          <t>KES 1,580,773</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>105.04%</t>
+          <t>158.08%</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KES -75,113</t>
+          <t>KES -580,773</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KES 184,910</t>
+          <t>KES 185,705</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>KES 1,750,023</t>
+          <t>KES 1,766,478</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>KES 260,023</t>
+          <t>KES 766,478</t>
         </is>
       </c>
     </row>
@@ -755,17 +755,17 @@
         </is>
       </c>
       <c r="B25" s="5" t="n">
-        <v>475220</v>
+        <v>485450</v>
       </c>
       <c r="C25" s="5" t="n">
-        <v>5949.5</v>
+        <v>6079.5</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>481169.5</v>
+        <v>491529.5</v>
       </c>
       <c r="E25" s="5" t="inlineStr">
         <is>
-          <t>32.29%</t>
+          <t>49.15%</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="E26" s="5" t="inlineStr">
         <is>
-          <t>23.66%</t>
+          <t>35.26%</t>
         </is>
       </c>
     </row>
@@ -807,7 +807,7 @@
       </c>
       <c r="E27" s="5" t="inlineStr">
         <is>
-          <t>18.79%</t>
+          <t>28.00%</t>
         </is>
       </c>
     </row>
@@ -828,7 +828,7 @@
       </c>
       <c r="E28" s="5" t="inlineStr">
         <is>
-          <t>11.97%</t>
+          <t>17.84%</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="E29" s="5" t="inlineStr">
         <is>
-          <t>6.14%</t>
+          <t>9.15%</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="E30" s="5" t="inlineStr">
         <is>
-          <t>2.10%</t>
+          <t>3.13%</t>
         </is>
       </c>
     </row>
@@ -891,7 +891,7 @@
       </c>
       <c r="E31" s="5" t="inlineStr">
         <is>
-          <t>1.49%</t>
+          <t>2.22%</t>
         </is>
       </c>
     </row>
@@ -912,7 +912,7 @@
       </c>
       <c r="E32" s="5" t="inlineStr">
         <is>
-          <t>0.73%</t>
+          <t>1.08%</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="E33" s="5" t="inlineStr">
         <is>
-          <t>0.68%</t>
+          <t>1.01%</t>
         </is>
       </c>
     </row>
@@ -954,7 +954,7 @@
       </c>
       <c r="E34" s="5" t="inlineStr">
         <is>
-          <t>0.35%</t>
+          <t>0.52%</t>
         </is>
       </c>
     </row>
@@ -972,7 +972,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I464"/>
+  <dimension ref="A1:I472"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20016,6 +20016,334 @@
         </is>
       </c>
       <c r="I464" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="6" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="B465" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C465" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D465" s="6" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="E465" s="6" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F465" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G465" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H465" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I465" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="6" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="B466" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C466" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D466" s="6" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E466" s="6" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F466" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G466" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H466" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I466" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="6" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="B467" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C467" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D467" s="6" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E467" s="6" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F467" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G467" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H467" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I467" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="6" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="B468" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C468" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D468" s="6" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="E468" s="6" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F468" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G468" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H468" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I468" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="5" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="B469" s="5" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C469" s="5" t="inlineStr">
+        <is>
+          <t>Finishing Materials</t>
+        </is>
+      </c>
+      <c r="D469" s="5" t="inlineStr">
+        <is>
+          <t>17ft faceboard 8X1 @ 90</t>
+        </is>
+      </c>
+      <c r="E469" s="5" t="n">
+        <v>1530</v>
+      </c>
+      <c r="F469" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="G469" s="5" t="n">
+        <v>1555</v>
+      </c>
+      <c r="H469" s="5" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I469" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="5" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="B470" s="5" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C470" s="5" t="inlineStr">
+        <is>
+          <t>Ceiling Materials</t>
+        </is>
+      </c>
+      <c r="D470" s="5" t="inlineStr">
+        <is>
+          <t>6 ceiling board 9mm @ 1050</t>
+        </is>
+      </c>
+      <c r="E470" s="5" t="n">
+        <v>6300</v>
+      </c>
+      <c r="F470" s="5" t="n">
+        <v>75</v>
+      </c>
+      <c r="G470" s="5" t="n">
+        <v>6375</v>
+      </c>
+      <c r="H470" s="5" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I470" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="5" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="B471" s="5" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C471" s="5" t="inlineStr">
+        <is>
+          <t>Finishing Materials</t>
+        </is>
+      </c>
+      <c r="D471" s="5" t="inlineStr">
+        <is>
+          <t>8 pcs Aluminium corners strip gold @ 250</t>
+        </is>
+      </c>
+      <c r="E471" s="5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F471" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="G471" s="5" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H471" s="5" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I471" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="5" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="B472" s="5" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C472" s="5" t="inlineStr">
+        <is>
+          <t>Ceiling Materials</t>
+        </is>
+      </c>
+      <c r="D472" s="5" t="inlineStr">
+        <is>
+          <t>Spacers 2.5mm 4 packets @ 100</t>
+        </is>
+      </c>
+      <c r="E472" s="5" t="n">
+        <v>400</v>
+      </c>
+      <c r="F472" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G472" s="5" t="n">
+        <v>405</v>
+      </c>
+      <c r="H472" s="5" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I472" s="5" t="inlineStr">
         <is>
           <t>PAID</t>
         </is>
@@ -20120,10 +20448,10 @@
         <v>25</v>
       </c>
       <c r="C6" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D6" t="n">
-        <v>1600</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="7">
@@ -20152,10 +20480,10 @@
         <v>75</v>
       </c>
       <c r="C8" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" t="n">
-        <v>1275</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="9">
@@ -20200,7 +20528,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="n">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D11" t="n">
         <v>2160</v>
@@ -20264,10 +20592,10 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D15" t="n">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16">
@@ -20310,7 +20638,7 @@
       </c>
       <c r="B20" s="8" t="inlineStr">
         <is>
-          <t>KES 16,771</t>
+          <t>KES 16,901</t>
         </is>
       </c>
     </row>
@@ -20514,7 +20842,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20717,15 +21045,95 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D12" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
     <row r="13">
-      <c r="A13" s="8" t="inlineStr">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D15" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
         <is>
           <t>Total Unpaid Labor:</t>
         </is>
       </c>
-      <c r="C13" s="8" t="inlineStr">
-        <is>
-          <t>KES 10,600</t>
+      <c r="C17" s="8" t="inlineStr">
+        <is>
+          <t>KES 15,900</t>
         </is>
       </c>
     </row>
@@ -20957,7 +21365,7 @@
         </is>
       </c>
       <c r="C15" s="11" t="n">
-        <v>37410</v>
+        <v>38205</v>
       </c>
     </row>
     <row r="17">
@@ -20968,7 +21376,7 @@
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>KES 184,910</t>
+          <t>KES 185,705</t>
         </is>
       </c>
     </row>
@@ -20987,7 +21395,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>KES 1,463,213</t>
+          <t>KES 1,473,573</t>
         </is>
       </c>
     </row>
@@ -21011,7 +21419,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>KES 10,600</t>
+          <t>KES 15,900</t>
         </is>
       </c>
     </row>
@@ -21023,7 +21431,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>KES 184,910</t>
+          <t>KES 185,705</t>
         </is>
       </c>
     </row>
@@ -21035,7 +21443,7 @@
       </c>
       <c r="B25" s="13" t="inlineStr">
         <is>
-          <t>KES 1,750,023</t>
+          <t>KES 1,766,478</t>
         </is>
       </c>
     </row>
@@ -21047,7 +21455,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>KES 1,490,000</t>
+          <t>KES 1,000,000</t>
         </is>
       </c>
     </row>
@@ -21059,7 +21467,7 @@
       </c>
       <c r="B27" s="14" t="inlineStr">
         <is>
-          <t>KES 260,023</t>
+          <t>KES 766,478</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Oct 22-23 labor and materials, remove cornis from pending
LABOR (UNPAID):
Oct 22: Jack 1,500 + Fundi 1&2 @ 1,300 each + 2 helpers @ 600 each = 5,300
Oct 23: Jack 1,500 + Fundi 1&2 @ 1,300 each + 2 helpers @ 600 each = 5,300

MATERIALS (PAID):
Oct 22: 58pcs gypsum cornis 13,340 + gypsum filler 2,150 + water 1,200 (UNPAID)
Oct 23: Redoxide 10kg 2,500 + 2 wire brushes 300

UPDATES:
- Removed cornis (15,000) from pending purchases since purchased
- Total spent: 1,492,074.50 (149.21% of budget)
- Unpaid labor now: 27,700 (up from 15,900)
- Pending purchases reduced: 170,225 (down from 187,475)
- Total additional funds needed: 781,299.50 (78.13% over budget)
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -503,7 +503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,7 +552,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KES 1,473,573</t>
+          <t>KES 1,492,074</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES -473,573</t>
+          <t>KES -492,074</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>147.36%</t>
+          <t>149.21%</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KES 16,901</t>
+          <t>KES 17,112</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>KES 15,900</t>
+          <t>KES 27,700</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KES 107,200</t>
+          <t>KES 119,000</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KES 1,580,773</t>
+          <t>KES 1,611,074</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>158.08%</t>
+          <t>161.11%</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KES -580,773</t>
+          <t>KES -611,074</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KES 185,705</t>
+          <t>KES 170,225</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>KES 1,766,478</t>
+          <t>KES 1,781,299</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>KES 766,478</t>
+          <t>KES 781,299</t>
         </is>
       </c>
     </row>
@@ -755,17 +755,17 @@
         </is>
       </c>
       <c r="B25" s="5" t="n">
-        <v>485450</v>
+        <v>490100</v>
       </c>
       <c r="C25" s="5" t="n">
-        <v>6079.5</v>
+        <v>6129.5</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>491529.5</v>
+        <v>496229.5</v>
       </c>
       <c r="E25" s="5" t="inlineStr">
         <is>
-          <t>49.15%</t>
+          <t>49.62%</t>
         </is>
       </c>
     </row>
@@ -797,17 +797,17 @@
         </is>
       </c>
       <c r="B27" s="5" t="n">
-        <v>276671</v>
+        <v>276971</v>
       </c>
       <c r="C27" s="5" t="n">
-        <v>3325.5</v>
+        <v>3330.5</v>
       </c>
       <c r="D27" s="5" t="n">
-        <v>279996.5</v>
+        <v>280301.5</v>
       </c>
       <c r="E27" s="5" t="inlineStr">
         <is>
-          <t>28.00%</t>
+          <t>28.03%</t>
         </is>
       </c>
     </row>
@@ -898,61 +898,82 @@
     <row r="32">
       <c r="A32" s="5" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Finishing &amp; Decoration</t>
         </is>
       </c>
       <c r="B32" s="5" t="n">
-        <v>10730</v>
+        <v>13340</v>
       </c>
       <c r="C32" s="5" t="n">
-        <v>115</v>
+        <v>156</v>
       </c>
       <c r="D32" s="5" t="n">
-        <v>10845</v>
+        <v>13496</v>
       </c>
       <c r="E32" s="5" t="inlineStr">
         <is>
-          <t>1.08%</t>
+          <t>1.35%</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="inlineStr">
         <is>
-          <t>Furniture &amp; Fixtures</t>
+          <t>Utilities</t>
         </is>
       </c>
       <c r="B33" s="5" t="n">
-        <v>10000</v>
+        <v>10730</v>
       </c>
       <c r="C33" s="5" t="n">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>10096</v>
+        <v>10845</v>
       </c>
       <c r="E33" s="5" t="inlineStr">
         <is>
-          <t>1.01%</t>
+          <t>1.08%</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="inlineStr">
         <is>
+          <t>Furniture &amp; Fixtures</t>
+        </is>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C34" s="5" t="n">
+        <v>96</v>
+      </c>
+      <c r="D34" s="5" t="n">
+        <v>10096</v>
+      </c>
+      <c r="E34" s="5" t="inlineStr">
+        <is>
+          <t>1.01%</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="inlineStr">
+        <is>
           <t>Utilities &amp; Services</t>
         </is>
       </c>
-      <c r="B34" s="5" t="n">
+      <c r="B35" s="5" t="n">
         <v>5100</v>
       </c>
-      <c r="C34" s="5" t="n">
+      <c r="C35" s="5" t="n">
         <v>75</v>
       </c>
-      <c r="D34" s="5" t="n">
+      <c r="D35" s="5" t="n">
         <v>5175</v>
       </c>
-      <c r="E34" s="5" t="inlineStr">
+      <c r="E35" s="5" t="inlineStr">
         <is>
           <t>0.52%</t>
         </is>
@@ -972,7 +993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I472"/>
+  <dimension ref="A1:I485"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20344,6 +20365,539 @@
         </is>
       </c>
       <c r="I472" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="6" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="B473" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C473" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D473" s="6" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="E473" s="6" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F473" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G473" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H473" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I473" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="6" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="B474" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C474" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D474" s="6" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E474" s="6" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F474" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G474" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H474" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I474" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="6" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="B475" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C475" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D475" s="6" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E475" s="6" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F475" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G475" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H475" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I475" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="6" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="B476" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C476" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D476" s="6" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="E476" s="6" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F476" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G476" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H476" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I476" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="5" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="B477" s="5" t="inlineStr">
+        <is>
+          <t>Finishing &amp; Decoration</t>
+        </is>
+      </c>
+      <c r="C477" s="5" t="inlineStr">
+        <is>
+          <t>Ceiling Materials</t>
+        </is>
+      </c>
+      <c r="D477" s="5" t="inlineStr">
+        <is>
+          <t>58pcs gypsum cornis @ 230</t>
+        </is>
+      </c>
+      <c r="E477" s="5" t="n">
+        <v>13340</v>
+      </c>
+      <c r="F477" s="5" t="n">
+        <v>156</v>
+      </c>
+      <c r="G477" s="5" t="n">
+        <v>13496</v>
+      </c>
+      <c r="H477" s="5" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I477" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="5" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="B478" s="5" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C478" s="5" t="inlineStr">
+        <is>
+          <t>Finishing Materials</t>
+        </is>
+      </c>
+      <c r="D478" s="5" t="inlineStr">
+        <is>
+          <t>1 bag gypsum filler @ 2150</t>
+        </is>
+      </c>
+      <c r="E478" s="5" t="n">
+        <v>2150</v>
+      </c>
+      <c r="F478" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="G478" s="5" t="n">
+        <v>2175</v>
+      </c>
+      <c r="H478" s="5" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I478" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="6" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="B479" s="6" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="C479" s="6" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="D479" s="6" t="inlineStr">
+        <is>
+          <t>Water - UNPAID</t>
+        </is>
+      </c>
+      <c r="E479" s="6" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F479" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G479" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H479" s="6" t="inlineStr">
+        <is>
+          <t>Water Supplier</t>
+        </is>
+      </c>
+      <c r="I479" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="6" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="B480" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C480" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D480" s="6" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="E480" s="6" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F480" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G480" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H480" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I480" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="6" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="B481" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C481" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D481" s="6" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E481" s="6" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F481" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G481" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H481" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I481" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="6" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="B482" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C482" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D482" s="6" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E482" s="6" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F482" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G482" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H482" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I482" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="6" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="B483" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C483" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D483" s="6" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="E483" s="6" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F483" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G483" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H483" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I483" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="5" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="B484" s="5" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C484" s="5" t="inlineStr">
+        <is>
+          <t>Paint &amp; Finishes</t>
+        </is>
+      </c>
+      <c r="D484" s="5" t="inlineStr">
+        <is>
+          <t>Redoxide 10kg @ 250</t>
+        </is>
+      </c>
+      <c r="E484" s="5" t="n">
+        <v>2500</v>
+      </c>
+      <c r="F484" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="G484" s="5" t="n">
+        <v>2525</v>
+      </c>
+      <c r="H484" s="5" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I484" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="5" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="B485" s="5" t="inlineStr">
+        <is>
+          <t>Hardware Items</t>
+        </is>
+      </c>
+      <c r="C485" s="5" t="inlineStr">
+        <is>
+          <t>Tools</t>
+        </is>
+      </c>
+      <c r="D485" s="5" t="inlineStr">
+        <is>
+          <t>2 wire brushes @ 150</t>
+        </is>
+      </c>
+      <c r="E485" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="F485" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G485" s="5" t="n">
+        <v>305</v>
+      </c>
+      <c r="H485" s="5" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I485" s="5" t="inlineStr">
         <is>
           <t>PAID</t>
         </is>
@@ -20448,10 +21002,10 @@
         <v>25</v>
       </c>
       <c r="C6" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D6" t="n">
-        <v>1650</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="7">
@@ -20528,7 +21082,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="n">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="D11" t="n">
         <v>2160</v>
@@ -20576,10 +21130,10 @@
         <v>156</v>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14" t="n">
-        <v>1404</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="15">
@@ -20592,10 +21146,10 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D15" t="n">
-        <v>285</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16">
@@ -20638,7 +21192,7 @@
       </c>
       <c r="B20" s="8" t="inlineStr">
         <is>
-          <t>KES 16,901</t>
+          <t>KES 17,112</t>
         </is>
       </c>
     </row>
@@ -20842,7 +21396,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21125,15 +21679,195 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
     <row r="17">
-      <c r="A17" s="8" t="inlineStr">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D18" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D19" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="B20" s="5" t="inlineStr">
+        <is>
+          <t>Water - UNPAID</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D20" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="C21" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D21" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D22" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D23" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D24" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="8" t="inlineStr">
         <is>
           <t>Total Unpaid Labor:</t>
         </is>
       </c>
-      <c r="C17" s="8" t="inlineStr">
-        <is>
-          <t>KES 15,900</t>
+      <c r="C26" s="8" t="inlineStr">
+        <is>
+          <t>KES 27,700</t>
         </is>
       </c>
     </row>
@@ -21151,7 +21885,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21221,16 +21955,16 @@
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>Finishing &amp; Decoration</t>
+          <t>Paint</t>
         </is>
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>Cornis</t>
+          <t>4 ltrs silk Lagoon</t>
         </is>
       </c>
       <c r="C6" s="5" t="n">
-        <v>15000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="7">
@@ -21241,11 +21975,11 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>4 ltrs silk Lagoon</t>
+          <t>20 ltrs silk Ivory</t>
         </is>
       </c>
       <c r="C7" s="5" t="n">
-        <v>3000</v>
+        <v>14700</v>
       </c>
     </row>
     <row r="8">
@@ -21256,26 +21990,26 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>20 ltrs silk Ivory</t>
+          <t>4 ltrs silk grey</t>
         </is>
       </c>
       <c r="C8" s="5" t="n">
-        <v>14700</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t>Paint</t>
+          <t>Paint - Outside</t>
         </is>
       </c>
       <c r="B9" s="5" t="inlineStr">
         <is>
-          <t>4 ltrs silk grey</t>
+          <t>4 ltrs Aquatech white</t>
         </is>
       </c>
       <c r="C9" s="5" t="n">
-        <v>3000</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="10">
@@ -21286,11 +22020,11 @@
       </c>
       <c r="B10" s="5" t="inlineStr">
         <is>
-          <t>4 ltrs Aquatech white</t>
+          <t>4 ltrs gloss black</t>
         </is>
       </c>
       <c r="C10" s="5" t="n">
-        <v>3200</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="11">
@@ -21301,11 +22035,11 @@
       </c>
       <c r="B11" s="5" t="inlineStr">
         <is>
-          <t>4 ltrs gloss black</t>
+          <t>4 ltrs weatherguard ivory</t>
         </is>
       </c>
       <c r="C11" s="5" t="n">
-        <v>1200</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="12">
@@ -21316,158 +22050,143 @@
       </c>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>4 ltrs weatherguard ivory</t>
+          <t>6 @ 4 ltrs weatherguard silicone @ 3200 each</t>
         </is>
       </c>
       <c r="C12" s="5" t="n">
-        <v>3200</v>
+        <v>19200</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t>Paint - Outside</t>
+          <t>Construction Work</t>
         </is>
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>6 @ 4 ltrs weatherguard silicone @ 3200 each</t>
+          <t>Veranda works and other pending concrete work</t>
         </is>
       </c>
       <c r="C13" s="5" t="n">
-        <v>19200</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="inlineStr">
-        <is>
-          <t>Construction Work</t>
-        </is>
-      </c>
-      <c r="B14" s="5" t="inlineStr">
-        <is>
-          <t>Veranda works and other pending concrete work</t>
-        </is>
-      </c>
-      <c r="C14" s="5" t="n">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="11" t="inlineStr">
+      <c r="A14" s="11" t="inlineStr">
         <is>
           <t>Miscellaneous &amp; Contingency</t>
         </is>
       </c>
-      <c r="B15" s="11" t="inlineStr">
+      <c r="B14" s="11" t="inlineStr">
         <is>
           <t>Estimated miscellaneous costs (15% of remaining work) - includes transport, food, accommodation, unexpected items</t>
         </is>
       </c>
-      <c r="C15" s="11" t="n">
-        <v>38205</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="8" t="inlineStr">
+      <c r="C14" s="11" t="n">
+        <v>37725</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8" t="inlineStr">
         <is>
           <t>Total Pending Purchases:</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
-        <is>
-          <t>KES 185,705</t>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>KES 170,225</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="12" t="inlineStr">
+        <is>
+          <t>SUMMARY:</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="12" t="inlineStr">
-        <is>
-          <t>SUMMARY:</t>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1. Already Spent (Paid):</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>KES 1,492,074</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1. Already Spent (Paid):</t>
+          <t>2. Outstanding Balances:</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>KES 1,473,573</t>
+          <t>KES 91,300</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2. Outstanding Balances:</t>
+          <t>3. Unpaid Labor:</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>KES 91,300</t>
+          <t>KES 27,700</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3. Unpaid Labor:</t>
+          <t>4. Pending Purchases:</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>KES 15,900</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>4. Pending Purchases:</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>KES 185,705</t>
+          <t>KES 170,225</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="13" t="inlineStr">
+        <is>
+          <t>TOTAL PROJECT COST:</t>
+        </is>
+      </c>
+      <c r="B24" s="13" t="inlineStr">
+        <is>
+          <t>KES 1,781,299</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="13" t="inlineStr">
-        <is>
-          <t>TOTAL PROJECT COST:</t>
-        </is>
-      </c>
-      <c r="B25" s="13" t="inlineStr">
-        <is>
-          <t>KES 1,766,478</t>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Current Budget:</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>KES 1,000,000</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Current Budget:</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>KES 1,000,000</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="14" t="inlineStr">
+      <c r="A26" s="14" t="inlineStr">
         <is>
           <t>Additional Funds Needed:</t>
         </is>
       </c>
-      <c r="B27" s="14" t="inlineStr">
-        <is>
-          <t>KES 766,478</t>
+      <c r="B26" s="14" t="inlineStr">
+        <is>
+          <t>KES 781,299</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add additional gypsum filler for Oct 23
- 1 bag gypsum filler @ 2,150 KES
- Total spent: 1,494,249.50 (149.42% of budget)
- Total transactions: 485
- Additional funds needed: 783,474.50 (78.35% over budget)
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -552,7 +552,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KES 1,492,074</t>
+          <t>KES 1,494,249</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES -492,074</t>
+          <t>KES -494,249</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>149.21%</t>
+          <t>149.42%</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KES 17,112</t>
+          <t>KES 17,137</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KES 1,611,074</t>
+          <t>KES 1,613,249</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>161.11%</t>
+          <t>161.32%</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KES -611,074</t>
+          <t>KES -613,249</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>KES 1,781,299</t>
+          <t>KES 1,783,474</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>KES 781,299</t>
+          <t>KES 783,474</t>
         </is>
       </c>
     </row>
@@ -755,17 +755,17 @@
         </is>
       </c>
       <c r="B25" s="5" t="n">
-        <v>490100</v>
+        <v>492250</v>
       </c>
       <c r="C25" s="5" t="n">
-        <v>6129.5</v>
+        <v>6154.5</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>496229.5</v>
+        <v>498404.5</v>
       </c>
       <c r="E25" s="5" t="inlineStr">
         <is>
-          <t>49.62%</t>
+          <t>49.84%</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I485"/>
+  <dimension ref="A1:I486"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20898,6 +20898,47 @@
         </is>
       </c>
       <c r="I485" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" s="5" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="B486" s="5" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C486" s="5" t="inlineStr">
+        <is>
+          <t>Finishing Materials</t>
+        </is>
+      </c>
+      <c r="D486" s="5" t="inlineStr">
+        <is>
+          <t>1 bag gypsum filler @ 2150</t>
+        </is>
+      </c>
+      <c r="E486" s="5" t="n">
+        <v>2150</v>
+      </c>
+      <c r="F486" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="G486" s="5" t="n">
+        <v>2175</v>
+      </c>
+      <c r="H486" s="5" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I486" s="5" t="inlineStr">
         <is>
           <t>PAID</t>
         </is>
@@ -21002,10 +21043,10 @@
         <v>25</v>
       </c>
       <c r="C6" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D6" t="n">
-        <v>1700</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="7">
@@ -21192,7 +21233,7 @@
       </c>
       <c r="B20" s="8" t="inlineStr">
         <is>
-          <t>KES 17,112</t>
+          <t>KES 17,137</t>
         </is>
       </c>
     </row>
@@ -22114,7 +22155,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KES 1,492,074</t>
+          <t>KES 1,494,249</t>
         </is>
       </c>
     </row>
@@ -22162,7 +22203,7 @@
       </c>
       <c r="B24" s="13" t="inlineStr">
         <is>
-          <t>KES 1,781,299</t>
+          <t>KES 1,783,474</t>
         </is>
       </c>
     </row>
@@ -22186,7 +22227,7 @@
       </c>
       <c r="B26" s="14" t="inlineStr">
         <is>
-          <t>KES 781,299</t>
+          <t>KES 783,474</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add painting work payment - 10,000 KES
- Payment for painting work: 10,000 KES (Oct 23)
- Reduced painter outstanding balance from 30,000 to 20,000
- Total spent: 1,504,345.50 (150.43% of budget)
- Outstanding balances reduced to: 81,300 (down from 91,300)
- Total pending reduced to: 277,725 (down from 289,225)
- Additional funds needed: 782,070.50 (78.21% over budget)
- Total transactions: 486
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -552,7 +552,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KES 1,494,249</t>
+          <t>KES 1,504,345</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES -494,249</t>
+          <t>KES -504,345</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>149.42%</t>
+          <t>150.43%</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KES 17,137</t>
+          <t>KES 17,233</t>
         </is>
       </c>
     </row>
@@ -607,7 +607,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>KES 91,300</t>
+          <t>KES 81,300</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KES 119,000</t>
+          <t>KES 109,000</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KES 1,613,249</t>
+          <t>KES 1,613,345</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>161.32%</t>
+          <t>161.33%</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KES -613,249</t>
+          <t>KES -613,345</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KES 170,225</t>
+          <t>KES 168,725</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>KES 1,783,474</t>
+          <t>KES 1,782,070</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>KES 783,474</t>
+          <t>KES 782,070</t>
         </is>
       </c>
     </row>
@@ -776,17 +776,17 @@
         </is>
       </c>
       <c r="B26" s="5" t="n">
-        <v>348600</v>
+        <v>358600</v>
       </c>
       <c r="C26" s="5" t="n">
-        <v>3988.5</v>
+        <v>4084.5</v>
       </c>
       <c r="D26" s="5" t="n">
-        <v>352588.5</v>
+        <v>362684.5</v>
       </c>
       <c r="E26" s="5" t="inlineStr">
         <is>
-          <t>35.26%</t>
+          <t>36.27%</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I486"/>
+  <dimension ref="A1:I487"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20939,6 +20939,47 @@
         </is>
       </c>
       <c r="I486" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" s="5" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="B487" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C487" s="5" t="inlineStr">
+        <is>
+          <t>Specialist Work</t>
+        </is>
+      </c>
+      <c r="D487" s="5" t="inlineStr">
+        <is>
+          <t>Payment for painting work</t>
+        </is>
+      </c>
+      <c r="E487" s="5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F487" s="5" t="n">
+        <v>96</v>
+      </c>
+      <c r="G487" s="5" t="n">
+        <v>10096</v>
+      </c>
+      <c r="H487" s="5" t="inlineStr">
+        <is>
+          <t>Painter</t>
+        </is>
+      </c>
+      <c r="I487" s="5" t="inlineStr">
         <is>
           <t>PAID</t>
         </is>
@@ -21027,10 +21068,10 @@
         <v>96</v>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="n">
-        <v>1728</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="6">
@@ -21233,7 +21274,7 @@
       </c>
       <c r="B20" s="8" t="inlineStr">
         <is>
-          <t>KES 17,137</t>
+          <t>KES 17,233</t>
         </is>
       </c>
     </row>
@@ -21359,11 +21400,11 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>Painting work - 30000</t>
+          <t>Painting work - 30000, paid 10000 on 23/10 = 20000 remaining</t>
         </is>
       </c>
       <c r="C7" s="5" t="n">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
@@ -21419,7 +21460,7 @@
       </c>
       <c r="C11" s="8" t="inlineStr">
         <is>
-          <t>KES 91,300</t>
+          <t>KES 81,300</t>
         </is>
       </c>
     </row>
@@ -22125,7 +22166,7 @@
         </is>
       </c>
       <c r="C14" s="11" t="n">
-        <v>37725</v>
+        <v>36225</v>
       </c>
     </row>
     <row r="16">
@@ -22136,7 +22177,7 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>KES 170,225</t>
+          <t>KES 168,725</t>
         </is>
       </c>
     </row>
@@ -22155,7 +22196,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KES 1,494,249</t>
+          <t>KES 1,504,345</t>
         </is>
       </c>
     </row>
@@ -22167,7 +22208,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>KES 91,300</t>
+          <t>KES 81,300</t>
         </is>
       </c>
     </row>
@@ -22191,7 +22232,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>KES 170,225</t>
+          <t>KES 168,725</t>
         </is>
       </c>
     </row>
@@ -22203,7 +22244,7 @@
       </c>
       <c r="B24" s="13" t="inlineStr">
         <is>
-          <t>KES 1,783,474</t>
+          <t>KES 1,782,070</t>
         </is>
       </c>
     </row>
@@ -22227,7 +22268,7 @@
       </c>
       <c r="B26" s="14" t="inlineStr">
         <is>
-          <t>KES 783,474</t>
+          <t>KES 782,070</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Oct 24 cement purchase - 15 bags Simba cement
- 15 bags Simba cement @ 720 = 10,800 KES
- Total spent: 1,515,301.50 (151.53% of budget)
- Building materials category increased to: 509,360.50
- Total transactions: 487
- Additional funds needed: 793,026.50 (79.30% over budget)
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -552,7 +552,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KES 1,504,345</t>
+          <t>KES 1,515,301</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES -504,345</t>
+          <t>KES -515,301</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>150.43%</t>
+          <t>151.53%</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KES 17,233</t>
+          <t>KES 17,389</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KES 1,613,345</t>
+          <t>KES 1,624,301</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>161.33%</t>
+          <t>162.43%</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KES -613,345</t>
+          <t>KES -624,301</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>KES 1,782,070</t>
+          <t>KES 1,793,026</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>KES 782,070</t>
+          <t>KES 793,026</t>
         </is>
       </c>
     </row>
@@ -755,17 +755,17 @@
         </is>
       </c>
       <c r="B25" s="5" t="n">
-        <v>492250</v>
+        <v>503050</v>
       </c>
       <c r="C25" s="5" t="n">
-        <v>6154.5</v>
+        <v>6310.5</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>498404.5</v>
+        <v>509360.5</v>
       </c>
       <c r="E25" s="5" t="inlineStr">
         <is>
-          <t>49.84%</t>
+          <t>50.94%</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I487"/>
+  <dimension ref="A1:I488"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20980,6 +20980,47 @@
         </is>
       </c>
       <c r="I487" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="5" t="inlineStr">
+        <is>
+          <t>24/10/2025</t>
+        </is>
+      </c>
+      <c r="B488" s="5" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C488" s="5" t="inlineStr">
+        <is>
+          <t>Cement &amp; Concrete</t>
+        </is>
+      </c>
+      <c r="D488" s="5" t="inlineStr">
+        <is>
+          <t>15 bags Simba cement @ 720</t>
+        </is>
+      </c>
+      <c r="E488" s="5" t="n">
+        <v>10800</v>
+      </c>
+      <c r="F488" s="5" t="n">
+        <v>156</v>
+      </c>
+      <c r="G488" s="5" t="n">
+        <v>10956</v>
+      </c>
+      <c r="H488" s="5" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I488" s="5" t="inlineStr">
         <is>
           <t>PAID</t>
         </is>
@@ -21212,10 +21253,10 @@
         <v>156</v>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" t="n">
-        <v>1560</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="15">
@@ -21274,7 +21315,7 @@
       </c>
       <c r="B20" s="8" t="inlineStr">
         <is>
-          <t>KES 17,233</t>
+          <t>KES 17,389</t>
         </is>
       </c>
     </row>
@@ -22196,7 +22237,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KES 1,504,345</t>
+          <t>KES 1,515,301</t>
         </is>
       </c>
     </row>
@@ -22244,7 +22285,7 @@
       </c>
       <c r="B24" s="13" t="inlineStr">
         <is>
-          <t>KES 1,782,070</t>
+          <t>KES 1,793,026</t>
         </is>
       </c>
     </row>
@@ -22268,7 +22309,7 @@
       </c>
       <c r="B26" s="14" t="inlineStr">
         <is>
-          <t>KES 782,070</t>
+          <t>KES 793,026</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add missing Friday Oct 24 labor entries - complete week
MISSING LABOR ADDED:
- Friday 24/10/2025: Jack 1,500 + Fundi 1&2 @ 1,300 each + 2 helpers @ 600 each = 5,300 KES (UNPAID)

COMPLETE WEEK NOW (Sun 19 - Sat 25):
✅ Sunday 19/10: 5,300 UNPAID
✅ Monday 20/10: 5,300 UNPAID
✅ Tuesday 21/10: 5,300 UNPAID
✅ Wednesday 22/10: 5,300 UNPAID + water 1,200 UNPAID
✅ Thursday 23/10: 5,300 UNPAID
✅ Friday 24/10: 5,300 UNPAID (ADDED)
✅ Saturday 25/10: 5,300 UNPAID + transport 600 UNPAID

UPDATED TOTALS:
- Unpaid labor: 38,900 (up from 33,600)
- Total pending: 290,605
- Total transactions: 497
- Additional funds needed: 806,916.50 (80.69% over budget)
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -552,7 +552,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KES 1,515,301</t>
+          <t>KES 1,516,311</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES -515,301</t>
+          <t>KES -516,311</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>151.53%</t>
+          <t>151.63%</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KES 17,389</t>
+          <t>KES 17,399</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>KES 27,700</t>
+          <t>KES 38,900</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KES 109,000</t>
+          <t>KES 120,200</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KES 1,624,301</t>
+          <t>KES 1,636,511</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>162.43%</t>
+          <t>163.65%</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KES -624,301</t>
+          <t>KES -636,511</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KES 168,725</t>
+          <t>KES 170,405</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>KES 1,793,026</t>
+          <t>KES 1,806,916</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>KES 793,026</t>
+          <t>KES 806,916</t>
         </is>
       </c>
     </row>
@@ -755,17 +755,17 @@
         </is>
       </c>
       <c r="B25" s="5" t="n">
-        <v>503050</v>
+        <v>504050</v>
       </c>
       <c r="C25" s="5" t="n">
-        <v>6310.5</v>
+        <v>6320.5</v>
       </c>
       <c r="D25" s="5" t="n">
-        <v>509360.5</v>
+        <v>510370.5</v>
       </c>
       <c r="E25" s="5" t="inlineStr">
         <is>
-          <t>50.94%</t>
+          <t>51.04%</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I488"/>
+  <dimension ref="A1:I498"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21021,6 +21021,416 @@
         </is>
       </c>
       <c r="I488" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="6" t="inlineStr">
+        <is>
+          <t>24/10/2025</t>
+        </is>
+      </c>
+      <c r="B489" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C489" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D489" s="6" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="E489" s="6" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F489" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G489" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H489" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I489" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="6" t="inlineStr">
+        <is>
+          <t>24/10/2025</t>
+        </is>
+      </c>
+      <c r="B490" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C490" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D490" s="6" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E490" s="6" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F490" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G490" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H490" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I490" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="6" t="inlineStr">
+        <is>
+          <t>24/10/2025</t>
+        </is>
+      </c>
+      <c r="B491" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C491" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D491" s="6" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E491" s="6" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F491" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G491" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H491" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I491" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="6" t="inlineStr">
+        <is>
+          <t>24/10/2025</t>
+        </is>
+      </c>
+      <c r="B492" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C492" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D492" s="6" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="E492" s="6" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F492" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G492" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H492" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I492" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="6" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B493" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C493" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D493" s="6" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="E493" s="6" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F493" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G493" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H493" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I493" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="6" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B494" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C494" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D494" s="6" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E494" s="6" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F494" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G494" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H494" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I494" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="6" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B495" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C495" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D495" s="6" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="E495" s="6" t="n">
+        <v>1300</v>
+      </c>
+      <c r="F495" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G495" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H495" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I495" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="6" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B496" s="6" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C496" s="6" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D496" s="6" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="E496" s="6" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F496" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G496" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H496" s="6" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I496" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="6" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B497" s="6" t="inlineStr">
+        <is>
+          <t>Transport &amp; Logistics</t>
+        </is>
+      </c>
+      <c r="C497" s="6" t="inlineStr">
+        <is>
+          <t>Worker Transport</t>
+        </is>
+      </c>
+      <c r="D497" s="6" t="inlineStr">
+        <is>
+          <t>Transport - UNPAID</t>
+        </is>
+      </c>
+      <c r="E497" s="6" t="n">
+        <v>600</v>
+      </c>
+      <c r="F497" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G497" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H497" s="6" t="inlineStr">
+        <is>
+          <t>Local Transport</t>
+        </is>
+      </c>
+      <c r="I497" s="7" t="inlineStr">
+        <is>
+          <t>UNPAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="5" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B498" s="5" t="inlineStr">
+        <is>
+          <t>Building Materials</t>
+        </is>
+      </c>
+      <c r="C498" s="5" t="inlineStr">
+        <is>
+          <t>Paint &amp; Finishes</t>
+        </is>
+      </c>
+      <c r="D498" s="5" t="inlineStr">
+        <is>
+          <t>5kg red oxide @ 200</t>
+        </is>
+      </c>
+      <c r="E498" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F498" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="G498" s="5" t="n">
+        <v>1010</v>
+      </c>
+      <c r="H498" s="5" t="inlineStr">
+        <is>
+          <t>Hardware Store</t>
+        </is>
+      </c>
+      <c r="I498" s="5" t="inlineStr">
         <is>
           <t>PAID</t>
         </is>
@@ -21205,7 +21615,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="n">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="D11" t="n">
         <v>2160</v>
@@ -21221,10 +21631,10 @@
         <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D12" t="n">
-        <v>900</v>
+        <v>910</v>
       </c>
     </row>
     <row r="13">
@@ -21315,7 +21725,7 @@
       </c>
       <c r="B20" s="8" t="inlineStr">
         <is>
-          <t>KES 17,389</t>
+          <t>KES 17,399</t>
         </is>
       </c>
     </row>
@@ -21519,7 +21929,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21982,15 +22392,195 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>24/10/2025</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D25" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
     <row r="26">
-      <c r="A26" s="8" t="inlineStr">
+      <c r="A26" s="5" t="inlineStr">
+        <is>
+          <t>24/10/2025</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C26" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D26" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t>24/10/2025</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D27" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="inlineStr">
+        <is>
+          <t>24/10/2025</t>
+        </is>
+      </c>
+      <c r="B28" s="5" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="C28" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D28" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B29" s="5" t="inlineStr">
+        <is>
+          <t>Jack - UNPAID</t>
+        </is>
+      </c>
+      <c r="C29" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D29" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C30" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D30" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B31" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - UNPAID</t>
+        </is>
+      </c>
+      <c r="C31" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="D31" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - UNPAID</t>
+        </is>
+      </c>
+      <c r="C32" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D32" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="inlineStr">
+        <is>
+          <t>Transport - UNPAID</t>
+        </is>
+      </c>
+      <c r="C33" s="5" t="n">
+        <v>600</v>
+      </c>
+      <c r="D33" s="10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="8" t="inlineStr">
         <is>
           <t>Total Unpaid Labor:</t>
         </is>
       </c>
-      <c r="C26" s="8" t="inlineStr">
-        <is>
-          <t>KES 27,700</t>
+      <c r="C35" s="8" t="inlineStr">
+        <is>
+          <t>KES 38,900</t>
         </is>
       </c>
     </row>
@@ -22207,7 +22797,7 @@
         </is>
       </c>
       <c r="C14" s="11" t="n">
-        <v>36225</v>
+        <v>37905</v>
       </c>
     </row>
     <row r="16">
@@ -22218,7 +22808,7 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>KES 168,725</t>
+          <t>KES 170,405</t>
         </is>
       </c>
     </row>
@@ -22237,7 +22827,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KES 1,515,301</t>
+          <t>KES 1,516,311</t>
         </is>
       </c>
     </row>
@@ -22261,7 +22851,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>KES 27,700</t>
+          <t>KES 38,900</t>
         </is>
       </c>
     </row>
@@ -22273,7 +22863,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>KES 168,725</t>
+          <t>KES 170,405</t>
         </is>
       </c>
     </row>
@@ -22285,7 +22875,7 @@
       </c>
       <c r="B24" s="13" t="inlineStr">
         <is>
-          <t>KES 1,793,026</t>
+          <t>KES 1,806,916</t>
         </is>
       </c>
     </row>
@@ -22309,7 +22899,7 @@
       </c>
       <c r="B26" s="14" t="inlineStr">
         <is>
-          <t>KES 793,026</t>
+          <t>KES 806,916</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Process Oct 25 payments - cleared all unpaid labor and balances
PAYMENTS MADE (25/10/2025):
1. Painting work: 7,000 KES (reduces painter balance 33K→16K)
2. Labor settlement: 39,935 KES (39,500 + 435 M-Pesa fees)
3. Cabinet specialist: 11,300 KES (clears balance to 0)

LABOR STATUS UPDATED:
- All UNPAID entries changed to 'PAID on 25/10'
- Sunday 19/10 to Saturday 25/10: ALL PAID
- Water and transport: PAID

UPDATED TOTALS:
- Total spent: 1,615,182.50 (161.52% of budget)
- Unpaid labor: 0 KES ✅ (was 39,500)
- Outstanding balances: 66,000 KES (was 94,300)
  * Painter: 16,000 KES (was 23,000)
  * Cabinet: 0 KES ✅ (was 11,300)
  * Others unchanged: Electrician 8K, Plumber 12K, Tile Fixer 30K
- Total pending: 228,275 KES (down from 291,295)
- Additional funds needed: 843,475 KES (84.35% over budget)
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -53,14 +53,6 @@
     </font>
     <font>
       <b val="1"/>
-      <color rgb="00CC0000"/>
-    </font>
-    <font>
-      <b val="1"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00E74C3C"/>
     </font>
     <font>
       <b val="1"/>
@@ -78,7 +70,7 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -89,12 +81,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00366092"/>
         <bgColor rgb="00366092"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFCCCC"/>
-        <bgColor rgb="00FFCCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -122,22 +108,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -552,7 +535,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KES 1,516,311</t>
+          <t>KES 1,615,182</t>
         </is>
       </c>
     </row>
@@ -564,7 +547,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES -516,311</t>
+          <t>KES -615,182</t>
         </is>
       </c>
     </row>
@@ -576,7 +559,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>151.63%</t>
+          <t>161.52%</t>
         </is>
       </c>
     </row>
@@ -588,7 +571,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KES 17,399</t>
+          <t>KES 18,535</t>
         </is>
       </c>
     </row>
@@ -607,7 +590,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>KES 81,300</t>
+          <t>KES 66,000</t>
         </is>
       </c>
     </row>
@@ -619,7 +602,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>KES 38,900</t>
+          <t>KES 0</t>
         </is>
       </c>
     </row>
@@ -631,7 +614,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KES 120,200</t>
+          <t>KES 66,000</t>
         </is>
       </c>
     </row>
@@ -643,7 +626,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KES 1,636,511</t>
+          <t>KES 1,681,182</t>
         </is>
       </c>
     </row>
@@ -655,7 +638,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>163.65%</t>
+          <t>168.12%</t>
         </is>
       </c>
     </row>
@@ -667,7 +650,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KES -636,511</t>
+          <t>KES -681,182</t>
         </is>
       </c>
     </row>
@@ -686,7 +669,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KES 170,405</t>
+          <t>KES 162,275</t>
         </is>
       </c>
     </row>
@@ -698,7 +681,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>KES 1,806,916</t>
+          <t>KES 1,843,457</t>
         </is>
       </c>
     </row>
@@ -710,7 +693,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>KES 806,916</t>
+          <t>KES 843,457</t>
         </is>
       </c>
     </row>
@@ -776,17 +759,17 @@
         </is>
       </c>
       <c r="B26" s="5" t="n">
-        <v>358600</v>
+        <v>453935</v>
       </c>
       <c r="C26" s="5" t="n">
-        <v>4084.5</v>
+        <v>5190.5</v>
       </c>
       <c r="D26" s="5" t="n">
-        <v>362684.5</v>
+        <v>459125.5</v>
       </c>
       <c r="E26" s="5" t="inlineStr">
         <is>
-          <t>36.27%</t>
+          <t>45.91%</t>
         </is>
       </c>
     </row>
@@ -881,17 +864,17 @@
         </is>
       </c>
       <c r="B31" s="5" t="n">
-        <v>21950</v>
+        <v>23150</v>
       </c>
       <c r="C31" s="5" t="n">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="D31" s="5" t="n">
-        <v>22200</v>
+        <v>23415</v>
       </c>
       <c r="E31" s="5" t="inlineStr">
         <is>
-          <t>2.22%</t>
+          <t>2.34%</t>
         </is>
       </c>
     </row>
@@ -923,17 +906,17 @@
         </is>
       </c>
       <c r="B33" s="5" t="n">
-        <v>10730</v>
+        <v>11930</v>
       </c>
       <c r="C33" s="5" t="n">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="D33" s="5" t="n">
-        <v>10845</v>
+        <v>12060</v>
       </c>
       <c r="E33" s="5" t="inlineStr">
         <is>
-          <t>1.08%</t>
+          <t>1.21%</t>
         </is>
       </c>
     </row>
@@ -993,7 +976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I498"/>
+  <dimension ref="A1:I501"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19633,330 +19616,330 @@
       </c>
     </row>
     <row r="455">
-      <c r="A455" s="6" t="inlineStr">
+      <c r="A455" s="5" t="inlineStr">
         <is>
           <t>19/10/2025</t>
         </is>
       </c>
-      <c r="B455" s="6" t="inlineStr">
+      <c r="B455" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C455" s="6" t="inlineStr">
+      <c r="C455" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D455" s="6" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="E455" s="6" t="n">
+      <c r="D455" s="5" t="inlineStr">
+        <is>
+          <t>Jack - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E455" s="5" t="n">
         <v>1500</v>
       </c>
-      <c r="F455" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G455" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H455" s="6" t="inlineStr">
+      <c r="F455" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G455" s="5" t="n">
+        <v>1515</v>
+      </c>
+      <c r="H455" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I455" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I455" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="456">
-      <c r="A456" s="6" t="inlineStr">
+      <c r="A456" s="5" t="inlineStr">
         <is>
           <t>19/10/2025</t>
         </is>
       </c>
-      <c r="B456" s="6" t="inlineStr">
+      <c r="B456" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C456" s="6" t="inlineStr">
+      <c r="C456" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D456" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E456" s="6" t="n">
+      <c r="D456" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E456" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F456" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G456" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H456" s="6" t="inlineStr">
+      <c r="F456" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G456" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H456" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I456" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I456" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="457">
-      <c r="A457" s="6" t="inlineStr">
+      <c r="A457" s="5" t="inlineStr">
         <is>
           <t>19/10/2025</t>
         </is>
       </c>
-      <c r="B457" s="6" t="inlineStr">
+      <c r="B457" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C457" s="6" t="inlineStr">
+      <c r="C457" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D457" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E457" s="6" t="n">
+      <c r="D457" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E457" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F457" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G457" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H457" s="6" t="inlineStr">
+      <c r="F457" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G457" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H457" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I457" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I457" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="458">
-      <c r="A458" s="6" t="inlineStr">
+      <c r="A458" s="5" t="inlineStr">
         <is>
           <t>19/10/2025</t>
         </is>
       </c>
-      <c r="B458" s="6" t="inlineStr">
+      <c r="B458" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C458" s="6" t="inlineStr">
+      <c r="C458" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D458" s="6" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="E458" s="6" t="n">
+      <c r="D458" s="5" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E458" s="5" t="n">
         <v>1200</v>
       </c>
-      <c r="F458" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G458" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H458" s="6" t="inlineStr">
+      <c r="F458" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G458" s="5" t="n">
+        <v>1215</v>
+      </c>
+      <c r="H458" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I458" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I458" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="459">
-      <c r="A459" s="6" t="inlineStr">
+      <c r="A459" s="5" t="inlineStr">
         <is>
           <t>20/10/2025</t>
         </is>
       </c>
-      <c r="B459" s="6" t="inlineStr">
+      <c r="B459" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C459" s="6" t="inlineStr">
+      <c r="C459" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D459" s="6" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="E459" s="6" t="n">
+      <c r="D459" s="5" t="inlineStr">
+        <is>
+          <t>Jack - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E459" s="5" t="n">
         <v>1500</v>
       </c>
-      <c r="F459" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G459" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H459" s="6" t="inlineStr">
+      <c r="F459" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G459" s="5" t="n">
+        <v>1515</v>
+      </c>
+      <c r="H459" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I459" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I459" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="460">
-      <c r="A460" s="6" t="inlineStr">
+      <c r="A460" s="5" t="inlineStr">
         <is>
           <t>20/10/2025</t>
         </is>
       </c>
-      <c r="B460" s="6" t="inlineStr">
+      <c r="B460" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C460" s="6" t="inlineStr">
+      <c r="C460" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D460" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E460" s="6" t="n">
+      <c r="D460" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E460" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F460" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G460" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H460" s="6" t="inlineStr">
+      <c r="F460" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G460" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H460" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I460" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I460" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="461">
-      <c r="A461" s="6" t="inlineStr">
+      <c r="A461" s="5" t="inlineStr">
         <is>
           <t>20/10/2025</t>
         </is>
       </c>
-      <c r="B461" s="6" t="inlineStr">
+      <c r="B461" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C461" s="6" t="inlineStr">
+      <c r="C461" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D461" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E461" s="6" t="n">
+      <c r="D461" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E461" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F461" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G461" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H461" s="6" t="inlineStr">
+      <c r="F461" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G461" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H461" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I461" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I461" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="462">
-      <c r="A462" s="6" t="inlineStr">
+      <c r="A462" s="5" t="inlineStr">
         <is>
           <t>20/10/2025</t>
         </is>
       </c>
-      <c r="B462" s="6" t="inlineStr">
+      <c r="B462" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C462" s="6" t="inlineStr">
+      <c r="C462" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D462" s="6" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="E462" s="6" t="n">
+      <c r="D462" s="5" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E462" s="5" t="n">
         <v>1200</v>
       </c>
-      <c r="F462" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G462" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H462" s="6" t="inlineStr">
+      <c r="F462" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G462" s="5" t="n">
+        <v>1215</v>
+      </c>
+      <c r="H462" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I462" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I462" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
@@ -20043,166 +20026,166 @@
       </c>
     </row>
     <row r="465">
-      <c r="A465" s="6" t="inlineStr">
+      <c r="A465" s="5" t="inlineStr">
         <is>
           <t>21/10/2025</t>
         </is>
       </c>
-      <c r="B465" s="6" t="inlineStr">
+      <c r="B465" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C465" s="6" t="inlineStr">
+      <c r="C465" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D465" s="6" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="E465" s="6" t="n">
+      <c r="D465" s="5" t="inlineStr">
+        <is>
+          <t>Jack - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E465" s="5" t="n">
         <v>1500</v>
       </c>
-      <c r="F465" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G465" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H465" s="6" t="inlineStr">
+      <c r="F465" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G465" s="5" t="n">
+        <v>1515</v>
+      </c>
+      <c r="H465" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I465" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I465" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="466">
-      <c r="A466" s="6" t="inlineStr">
+      <c r="A466" s="5" t="inlineStr">
         <is>
           <t>21/10/2025</t>
         </is>
       </c>
-      <c r="B466" s="6" t="inlineStr">
+      <c r="B466" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C466" s="6" t="inlineStr">
+      <c r="C466" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D466" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E466" s="6" t="n">
+      <c r="D466" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E466" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F466" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G466" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H466" s="6" t="inlineStr">
+      <c r="F466" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G466" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H466" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I466" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I466" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="467">
-      <c r="A467" s="6" t="inlineStr">
+      <c r="A467" s="5" t="inlineStr">
         <is>
           <t>21/10/2025</t>
         </is>
       </c>
-      <c r="B467" s="6" t="inlineStr">
+      <c r="B467" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C467" s="6" t="inlineStr">
+      <c r="C467" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D467" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E467" s="6" t="n">
+      <c r="D467" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E467" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F467" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G467" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H467" s="6" t="inlineStr">
+      <c r="F467" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G467" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H467" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I467" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I467" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="468">
-      <c r="A468" s="6" t="inlineStr">
+      <c r="A468" s="5" t="inlineStr">
         <is>
           <t>21/10/2025</t>
         </is>
       </c>
-      <c r="B468" s="6" t="inlineStr">
+      <c r="B468" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C468" s="6" t="inlineStr">
+      <c r="C468" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D468" s="6" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="E468" s="6" t="n">
+      <c r="D468" s="5" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E468" s="5" t="n">
         <v>1200</v>
       </c>
-      <c r="F468" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G468" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H468" s="6" t="inlineStr">
+      <c r="F468" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G468" s="5" t="n">
+        <v>1215</v>
+      </c>
+      <c r="H468" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I468" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I468" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
@@ -20371,166 +20354,166 @@
       </c>
     </row>
     <row r="473">
-      <c r="A473" s="6" t="inlineStr">
+      <c r="A473" s="5" t="inlineStr">
         <is>
           <t>22/10/2025</t>
         </is>
       </c>
-      <c r="B473" s="6" t="inlineStr">
+      <c r="B473" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C473" s="6" t="inlineStr">
+      <c r="C473" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D473" s="6" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="E473" s="6" t="n">
+      <c r="D473" s="5" t="inlineStr">
+        <is>
+          <t>Jack - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E473" s="5" t="n">
         <v>1500</v>
       </c>
-      <c r="F473" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G473" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H473" s="6" t="inlineStr">
+      <c r="F473" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G473" s="5" t="n">
+        <v>1515</v>
+      </c>
+      <c r="H473" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I473" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I473" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="474">
-      <c r="A474" s="6" t="inlineStr">
+      <c r="A474" s="5" t="inlineStr">
         <is>
           <t>22/10/2025</t>
         </is>
       </c>
-      <c r="B474" s="6" t="inlineStr">
+      <c r="B474" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C474" s="6" t="inlineStr">
+      <c r="C474" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D474" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E474" s="6" t="n">
+      <c r="D474" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E474" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F474" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G474" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H474" s="6" t="inlineStr">
+      <c r="F474" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G474" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H474" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I474" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I474" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="475">
-      <c r="A475" s="6" t="inlineStr">
+      <c r="A475" s="5" t="inlineStr">
         <is>
           <t>22/10/2025</t>
         </is>
       </c>
-      <c r="B475" s="6" t="inlineStr">
+      <c r="B475" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C475" s="6" t="inlineStr">
+      <c r="C475" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D475" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E475" s="6" t="n">
+      <c r="D475" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E475" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F475" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G475" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H475" s="6" t="inlineStr">
+      <c r="F475" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G475" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H475" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I475" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I475" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="476">
-      <c r="A476" s="6" t="inlineStr">
+      <c r="A476" s="5" t="inlineStr">
         <is>
           <t>22/10/2025</t>
         </is>
       </c>
-      <c r="B476" s="6" t="inlineStr">
+      <c r="B476" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C476" s="6" t="inlineStr">
+      <c r="C476" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D476" s="6" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="E476" s="6" t="n">
+      <c r="D476" s="5" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E476" s="5" t="n">
         <v>1200</v>
       </c>
-      <c r="F476" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G476" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H476" s="6" t="inlineStr">
+      <c r="F476" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G476" s="5" t="n">
+        <v>1215</v>
+      </c>
+      <c r="H476" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I476" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I476" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
@@ -20617,207 +20600,207 @@
       </c>
     </row>
     <row r="479">
-      <c r="A479" s="6" t="inlineStr">
+      <c r="A479" s="5" t="inlineStr">
         <is>
           <t>22/10/2025</t>
         </is>
       </c>
-      <c r="B479" s="6" t="inlineStr">
+      <c r="B479" s="5" t="inlineStr">
         <is>
           <t>Utilities</t>
         </is>
       </c>
-      <c r="C479" s="6" t="inlineStr">
+      <c r="C479" s="5" t="inlineStr">
         <is>
           <t>Water</t>
         </is>
       </c>
-      <c r="D479" s="6" t="inlineStr">
-        <is>
-          <t>Water - UNPAID</t>
-        </is>
-      </c>
-      <c r="E479" s="6" t="n">
+      <c r="D479" s="5" t="inlineStr">
+        <is>
+          <t>Water - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E479" s="5" t="n">
         <v>1200</v>
       </c>
-      <c r="F479" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G479" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H479" s="6" t="inlineStr">
+      <c r="F479" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G479" s="5" t="n">
+        <v>1215</v>
+      </c>
+      <c r="H479" s="5" t="inlineStr">
         <is>
           <t>Water Supplier</t>
         </is>
       </c>
-      <c r="I479" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I479" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="480">
-      <c r="A480" s="6" t="inlineStr">
+      <c r="A480" s="5" t="inlineStr">
         <is>
           <t>23/10/2025</t>
         </is>
       </c>
-      <c r="B480" s="6" t="inlineStr">
+      <c r="B480" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C480" s="6" t="inlineStr">
+      <c r="C480" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D480" s="6" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="E480" s="6" t="n">
+      <c r="D480" s="5" t="inlineStr">
+        <is>
+          <t>Jack - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E480" s="5" t="n">
         <v>1500</v>
       </c>
-      <c r="F480" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G480" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H480" s="6" t="inlineStr">
+      <c r="F480" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G480" s="5" t="n">
+        <v>1515</v>
+      </c>
+      <c r="H480" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I480" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I480" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="481">
-      <c r="A481" s="6" t="inlineStr">
+      <c r="A481" s="5" t="inlineStr">
         <is>
           <t>23/10/2025</t>
         </is>
       </c>
-      <c r="B481" s="6" t="inlineStr">
+      <c r="B481" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C481" s="6" t="inlineStr">
+      <c r="C481" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D481" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E481" s="6" t="n">
+      <c r="D481" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E481" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F481" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G481" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H481" s="6" t="inlineStr">
+      <c r="F481" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G481" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H481" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I481" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I481" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="482">
-      <c r="A482" s="6" t="inlineStr">
+      <c r="A482" s="5" t="inlineStr">
         <is>
           <t>23/10/2025</t>
         </is>
       </c>
-      <c r="B482" s="6" t="inlineStr">
+      <c r="B482" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C482" s="6" t="inlineStr">
+      <c r="C482" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D482" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E482" s="6" t="n">
+      <c r="D482" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E482" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F482" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G482" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H482" s="6" t="inlineStr">
+      <c r="F482" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G482" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H482" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I482" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I482" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="483">
-      <c r="A483" s="6" t="inlineStr">
+      <c r="A483" s="5" t="inlineStr">
         <is>
           <t>23/10/2025</t>
         </is>
       </c>
-      <c r="B483" s="6" t="inlineStr">
+      <c r="B483" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C483" s="6" t="inlineStr">
+      <c r="C483" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D483" s="6" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="E483" s="6" t="n">
+      <c r="D483" s="5" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E483" s="5" t="n">
         <v>1200</v>
       </c>
-      <c r="F483" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G483" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H483" s="6" t="inlineStr">
+      <c r="F483" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G483" s="5" t="n">
+        <v>1215</v>
+      </c>
+      <c r="H483" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I483" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I483" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
@@ -21027,371 +21010,371 @@
       </c>
     </row>
     <row r="489">
-      <c r="A489" s="6" t="inlineStr">
+      <c r="A489" s="5" t="inlineStr">
         <is>
           <t>24/10/2025</t>
         </is>
       </c>
-      <c r="B489" s="6" t="inlineStr">
+      <c r="B489" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C489" s="6" t="inlineStr">
+      <c r="C489" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D489" s="6" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="E489" s="6" t="n">
+      <c r="D489" s="5" t="inlineStr">
+        <is>
+          <t>Jack - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E489" s="5" t="n">
         <v>1500</v>
       </c>
-      <c r="F489" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G489" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H489" s="6" t="inlineStr">
+      <c r="F489" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G489" s="5" t="n">
+        <v>1515</v>
+      </c>
+      <c r="H489" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I489" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I489" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="490">
-      <c r="A490" s="6" t="inlineStr">
+      <c r="A490" s="5" t="inlineStr">
         <is>
           <t>24/10/2025</t>
         </is>
       </c>
-      <c r="B490" s="6" t="inlineStr">
+      <c r="B490" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C490" s="6" t="inlineStr">
+      <c r="C490" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D490" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E490" s="6" t="n">
+      <c r="D490" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E490" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F490" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G490" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H490" s="6" t="inlineStr">
+      <c r="F490" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G490" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H490" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I490" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I490" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="491">
-      <c r="A491" s="6" t="inlineStr">
+      <c r="A491" s="5" t="inlineStr">
         <is>
           <t>24/10/2025</t>
         </is>
       </c>
-      <c r="B491" s="6" t="inlineStr">
+      <c r="B491" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C491" s="6" t="inlineStr">
+      <c r="C491" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D491" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E491" s="6" t="n">
+      <c r="D491" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E491" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F491" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G491" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H491" s="6" t="inlineStr">
+      <c r="F491" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G491" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H491" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I491" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I491" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="492">
-      <c r="A492" s="6" t="inlineStr">
+      <c r="A492" s="5" t="inlineStr">
         <is>
           <t>24/10/2025</t>
         </is>
       </c>
-      <c r="B492" s="6" t="inlineStr">
+      <c r="B492" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C492" s="6" t="inlineStr">
+      <c r="C492" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D492" s="6" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="E492" s="6" t="n">
+      <c r="D492" s="5" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E492" s="5" t="n">
         <v>1200</v>
       </c>
-      <c r="F492" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G492" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H492" s="6" t="inlineStr">
+      <c r="F492" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G492" s="5" t="n">
+        <v>1215</v>
+      </c>
+      <c r="H492" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I492" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I492" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="493">
-      <c r="A493" s="6" t="inlineStr">
+      <c r="A493" s="5" t="inlineStr">
         <is>
           <t>25/10/2025</t>
         </is>
       </c>
-      <c r="B493" s="6" t="inlineStr">
+      <c r="B493" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C493" s="6" t="inlineStr">
+      <c r="C493" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D493" s="6" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="E493" s="6" t="n">
+      <c r="D493" s="5" t="inlineStr">
+        <is>
+          <t>Jack - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E493" s="5" t="n">
         <v>1500</v>
       </c>
-      <c r="F493" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G493" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H493" s="6" t="inlineStr">
+      <c r="F493" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G493" s="5" t="n">
+        <v>1515</v>
+      </c>
+      <c r="H493" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I493" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I493" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="494">
-      <c r="A494" s="6" t="inlineStr">
+      <c r="A494" s="5" t="inlineStr">
         <is>
           <t>25/10/2025</t>
         </is>
       </c>
-      <c r="B494" s="6" t="inlineStr">
+      <c r="B494" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C494" s="6" t="inlineStr">
+      <c r="C494" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D494" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E494" s="6" t="n">
+      <c r="D494" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 1 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E494" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F494" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G494" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H494" s="6" t="inlineStr">
+      <c r="F494" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G494" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H494" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I494" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I494" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="495">
-      <c r="A495" s="6" t="inlineStr">
+      <c r="A495" s="5" t="inlineStr">
         <is>
           <t>25/10/2025</t>
         </is>
       </c>
-      <c r="B495" s="6" t="inlineStr">
+      <c r="B495" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C495" s="6" t="inlineStr">
+      <c r="C495" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D495" s="6" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="E495" s="6" t="n">
+      <c r="D495" s="5" t="inlineStr">
+        <is>
+          <t>Fundi 2 - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E495" s="5" t="n">
         <v>1300</v>
       </c>
-      <c r="F495" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G495" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H495" s="6" t="inlineStr">
+      <c r="F495" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G495" s="5" t="n">
+        <v>1315</v>
+      </c>
+      <c r="H495" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I495" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I495" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="496">
-      <c r="A496" s="6" t="inlineStr">
+      <c r="A496" s="5" t="inlineStr">
         <is>
           <t>25/10/2025</t>
         </is>
       </c>
-      <c r="B496" s="6" t="inlineStr">
+      <c r="B496" s="5" t="inlineStr">
         <is>
           <t>Labor Costs</t>
         </is>
       </c>
-      <c r="C496" s="6" t="inlineStr">
+      <c r="C496" s="5" t="inlineStr">
         <is>
           <t>Daily Labor</t>
         </is>
       </c>
-      <c r="D496" s="6" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="E496" s="6" t="n">
+      <c r="D496" s="5" t="inlineStr">
+        <is>
+          <t>2 helpers @ 600 each - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E496" s="5" t="n">
         <v>1200</v>
       </c>
-      <c r="F496" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G496" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H496" s="6" t="inlineStr">
+      <c r="F496" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G496" s="5" t="n">
+        <v>1215</v>
+      </c>
+      <c r="H496" s="5" t="inlineStr">
         <is>
           <t>Worker</t>
         </is>
       </c>
-      <c r="I496" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I496" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
     <row r="497">
-      <c r="A497" s="6" t="inlineStr">
+      <c r="A497" s="5" t="inlineStr">
         <is>
           <t>25/10/2025</t>
         </is>
       </c>
-      <c r="B497" s="6" t="inlineStr">
+      <c r="B497" s="5" t="inlineStr">
         <is>
           <t>Transport &amp; Logistics</t>
         </is>
       </c>
-      <c r="C497" s="6" t="inlineStr">
+      <c r="C497" s="5" t="inlineStr">
         <is>
           <t>Worker Transport</t>
         </is>
       </c>
-      <c r="D497" s="6" t="inlineStr">
-        <is>
-          <t>Transport - UNPAID</t>
-        </is>
-      </c>
-      <c r="E497" s="6" t="n">
-        <v>600</v>
-      </c>
-      <c r="F497" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G497" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H497" s="6" t="inlineStr">
+      <c r="D497" s="5" t="inlineStr">
+        <is>
+          <t>Transport - PAID on 25/10</t>
+        </is>
+      </c>
+      <c r="E497" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F497" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G497" s="5" t="n">
+        <v>1215</v>
+      </c>
+      <c r="H497" s="5" t="inlineStr">
         <is>
           <t>Local Transport</t>
         </is>
       </c>
-      <c r="I497" s="7" t="inlineStr">
-        <is>
-          <t>UNPAID</t>
+      <c r="I497" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
         </is>
       </c>
     </row>
@@ -21431,6 +21414,129 @@
         </is>
       </c>
       <c r="I498" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="5" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B499" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C499" s="5" t="inlineStr">
+        <is>
+          <t>Specialist Work</t>
+        </is>
+      </c>
+      <c r="D499" s="5" t="inlineStr">
+        <is>
+          <t>Payment to reduce painting balance</t>
+        </is>
+      </c>
+      <c r="E499" s="5" t="n">
+        <v>7000</v>
+      </c>
+      <c r="F499" s="5" t="n">
+        <v>75</v>
+      </c>
+      <c r="G499" s="5" t="n">
+        <v>7075</v>
+      </c>
+      <c r="H499" s="5" t="inlineStr">
+        <is>
+          <t>Painter</t>
+        </is>
+      </c>
+      <c r="I499" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="5" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B500" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C500" s="5" t="inlineStr">
+        <is>
+          <t>Daily Labor</t>
+        </is>
+      </c>
+      <c r="D500" s="5" t="inlineStr">
+        <is>
+          <t>Payment for unpaid labor, water and transport (39500 + 435 M-Pesa fees)</t>
+        </is>
+      </c>
+      <c r="E500" s="5" t="n">
+        <v>39935</v>
+      </c>
+      <c r="F500" s="5" t="n">
+        <v>455</v>
+      </c>
+      <c r="G500" s="5" t="n">
+        <v>40390</v>
+      </c>
+      <c r="H500" s="5" t="inlineStr">
+        <is>
+          <t>Worker</t>
+        </is>
+      </c>
+      <c r="I500" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="5" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B501" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C501" s="5" t="inlineStr">
+        <is>
+          <t>Specialist Work</t>
+        </is>
+      </c>
+      <c r="D501" s="5" t="inlineStr">
+        <is>
+          <t>Clear cabinet specialist balance</t>
+        </is>
+      </c>
+      <c r="E501" s="5" t="n">
+        <v>11300</v>
+      </c>
+      <c r="F501" s="5" t="n">
+        <v>156</v>
+      </c>
+      <c r="G501" s="5" t="n">
+        <v>11456</v>
+      </c>
+      <c r="H501" s="5" t="inlineStr">
+        <is>
+          <t>Cabinet Specialist</t>
+        </is>
+      </c>
+      <c r="I501" s="5" t="inlineStr">
         <is>
           <t>PAID</t>
         </is>
@@ -21481,29 +21587,29 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="inlineStr">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Fee Structure</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="inlineStr">
+      <c r="A4" s="7" t="inlineStr">
         <is>
           <t>Amount Range</t>
         </is>
       </c>
-      <c r="B4" s="9" t="inlineStr">
+      <c r="B4" s="7" t="inlineStr">
         <is>
           <t>Fee (KES)</t>
         </is>
       </c>
-      <c r="C4" s="9" t="inlineStr">
+      <c r="C4" s="7" t="inlineStr">
         <is>
           <t>Transactions</t>
         </is>
       </c>
-      <c r="D4" s="9" t="inlineStr">
+      <c r="D4" s="7" t="inlineStr">
         <is>
           <t>Total Fees</t>
         </is>
@@ -21567,10 +21673,10 @@
         <v>75</v>
       </c>
       <c r="C8" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" t="n">
-        <v>1350</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="9">
@@ -21599,10 +21705,10 @@
         <v>455</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>1365</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="11">
@@ -21615,10 +21721,10 @@
         <v>15</v>
       </c>
       <c r="C11" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D11" t="n">
-        <v>2160</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="12">
@@ -21631,7 +21737,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" t="n">
         <v>910</v>
@@ -21663,10 +21769,10 @@
         <v>156</v>
       </c>
       <c r="C14" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" t="n">
-        <v>1716</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="15">
@@ -21723,9 +21829,9 @@
           <t>Total M-Pesa Fees:</t>
         </is>
       </c>
-      <c r="B20" s="8" t="inlineStr">
-        <is>
-          <t>KES 17,399</t>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t>KES 18,535</t>
         </is>
       </c>
     </row>
@@ -21851,11 +21957,11 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>Painting work - 30000, paid 10000 on 23/10 = 20000 remaining</t>
+          <t>Painting work - 33000, paid 10000 on 23/10 + 7000 on 25/10 = 16000 remaining</t>
         </is>
       </c>
       <c r="C7" s="5" t="n">
-        <v>20000</v>
+        <v>16000</v>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
@@ -21871,15 +21977,15 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>Original 16000 + unpaid work (3000 doors + 1800 curtain rods + 500 tip), paid 10000 down = 11300 remaining</t>
+          <t>Original 16000 + unpaid work (3000 doors + 1800 curtain rods + 500 tip), paid 10000 down + 11300 final = 0 remaining</t>
         </is>
       </c>
       <c r="C8" s="5" t="n">
-        <v>11300</v>
+        <v>0</v>
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>To be scheduled</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -21904,14 +22010,14 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="inlineStr">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>Total Outstanding:</t>
         </is>
       </c>
-      <c r="C11" s="8" t="inlineStr">
-        <is>
-          <t>KES 81,300</t>
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <t>KES 66,000</t>
         </is>
       </c>
     </row>
@@ -21929,7 +22035,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21972,615 +22078,15 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="5" t="inlineStr">
-        <is>
-          <t>19/10/2025</t>
-        </is>
-      </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D4" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
     <row r="5">
-      <c r="A5" s="5" t="inlineStr">
-        <is>
-          <t>19/10/2025</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D5" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5" t="inlineStr">
-        <is>
-          <t>19/10/2025</t>
-        </is>
-      </c>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D6" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>19/10/2025</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D7" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B8" s="5" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="C8" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D8" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B9" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D9" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="5" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B10" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C10" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D10" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="inlineStr">
-        <is>
-          <t>20/10/2025</t>
-        </is>
-      </c>
-      <c r="B11" s="5" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="C11" s="5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D11" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="inlineStr">
-        <is>
-          <t>21/10/2025</t>
-        </is>
-      </c>
-      <c r="B12" s="5" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="C12" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D12" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="inlineStr">
-        <is>
-          <t>21/10/2025</t>
-        </is>
-      </c>
-      <c r="B13" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C13" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D13" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="inlineStr">
-        <is>
-          <t>21/10/2025</t>
-        </is>
-      </c>
-      <c r="B14" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C14" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D14" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="inlineStr">
-        <is>
-          <t>21/10/2025</t>
-        </is>
-      </c>
-      <c r="B15" s="5" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="C15" s="5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D15" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="5" t="inlineStr">
-        <is>
-          <t>22/10/2025</t>
-        </is>
-      </c>
-      <c r="B16" s="5" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="C16" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D16" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="inlineStr">
-        <is>
-          <t>22/10/2025</t>
-        </is>
-      </c>
-      <c r="B17" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C17" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D17" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="5" t="inlineStr">
-        <is>
-          <t>22/10/2025</t>
-        </is>
-      </c>
-      <c r="B18" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C18" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D18" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="inlineStr">
-        <is>
-          <t>22/10/2025</t>
-        </is>
-      </c>
-      <c r="B19" s="5" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="C19" s="5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D19" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="5" t="inlineStr">
-        <is>
-          <t>22/10/2025</t>
-        </is>
-      </c>
-      <c r="B20" s="5" t="inlineStr">
-        <is>
-          <t>Water - UNPAID</t>
-        </is>
-      </c>
-      <c r="C20" s="5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D20" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="inlineStr">
-        <is>
-          <t>23/10/2025</t>
-        </is>
-      </c>
-      <c r="B21" s="5" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="C21" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D21" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="5" t="inlineStr">
-        <is>
-          <t>23/10/2025</t>
-        </is>
-      </c>
-      <c r="B22" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C22" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D22" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="inlineStr">
-        <is>
-          <t>23/10/2025</t>
-        </is>
-      </c>
-      <c r="B23" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C23" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D23" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="5" t="inlineStr">
-        <is>
-          <t>23/10/2025</t>
-        </is>
-      </c>
-      <c r="B24" s="5" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="C24" s="5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D24" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="inlineStr">
-        <is>
-          <t>24/10/2025</t>
-        </is>
-      </c>
-      <c r="B25" s="5" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="C25" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D25" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="5" t="inlineStr">
-        <is>
-          <t>24/10/2025</t>
-        </is>
-      </c>
-      <c r="B26" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C26" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D26" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="5" t="inlineStr">
-        <is>
-          <t>24/10/2025</t>
-        </is>
-      </c>
-      <c r="B27" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C27" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D27" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="5" t="inlineStr">
-        <is>
-          <t>24/10/2025</t>
-        </is>
-      </c>
-      <c r="B28" s="5" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="C28" s="5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D28" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="5" t="inlineStr">
-        <is>
-          <t>25/10/2025</t>
-        </is>
-      </c>
-      <c r="B29" s="5" t="inlineStr">
-        <is>
-          <t>Jack - UNPAID</t>
-        </is>
-      </c>
-      <c r="C29" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D29" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="5" t="inlineStr">
-        <is>
-          <t>25/10/2025</t>
-        </is>
-      </c>
-      <c r="B30" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 1 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C30" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D30" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="5" t="inlineStr">
-        <is>
-          <t>25/10/2025</t>
-        </is>
-      </c>
-      <c r="B31" s="5" t="inlineStr">
-        <is>
-          <t>Fundi 2 - UNPAID</t>
-        </is>
-      </c>
-      <c r="C31" s="5" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D31" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="5" t="inlineStr">
-        <is>
-          <t>25/10/2025</t>
-        </is>
-      </c>
-      <c r="B32" s="5" t="inlineStr">
-        <is>
-          <t>2 helpers @ 600 each - UNPAID</t>
-        </is>
-      </c>
-      <c r="C32" s="5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D32" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="5" t="inlineStr">
-        <is>
-          <t>25/10/2025</t>
-        </is>
-      </c>
-      <c r="B33" s="5" t="inlineStr">
-        <is>
-          <t>Transport - UNPAID</t>
-        </is>
-      </c>
-      <c r="C33" s="5" t="n">
-        <v>600</v>
-      </c>
-      <c r="D33" s="10" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="8" t="inlineStr">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Total Unpaid Labor:</t>
         </is>
       </c>
-      <c r="C35" s="8" t="inlineStr">
-        <is>
-          <t>KES 38,900</t>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>KES 0</t>
         </is>
       </c>
     </row>
@@ -22786,34 +22292,34 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="inlineStr">
+      <c r="A14" s="8" t="inlineStr">
         <is>
           <t>Miscellaneous &amp; Contingency</t>
         </is>
       </c>
-      <c r="B14" s="11" t="inlineStr">
+      <c r="B14" s="8" t="inlineStr">
         <is>
           <t>Estimated miscellaneous costs (15% of remaining work) - includes transport, food, accommodation, unexpected items</t>
         </is>
       </c>
-      <c r="C14" s="11" t="n">
-        <v>37905</v>
+      <c r="C14" s="8" t="n">
+        <v>29775</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="8" t="inlineStr">
+      <c r="A16" s="6" t="inlineStr">
         <is>
           <t>Total Pending Purchases:</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>KES 170,405</t>
+          <t>KES 162,275</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="12" t="inlineStr">
+      <c r="A18" s="9" t="inlineStr">
         <is>
           <t>SUMMARY:</t>
         </is>
@@ -22827,7 +22333,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KES 1,516,311</t>
+          <t>KES 1,615,182</t>
         </is>
       </c>
     </row>
@@ -22839,7 +22345,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>KES 81,300</t>
+          <t>KES 66,000</t>
         </is>
       </c>
     </row>
@@ -22851,7 +22357,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>KES 38,900</t>
+          <t>KES 0</t>
         </is>
       </c>
     </row>
@@ -22863,19 +22369,19 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>KES 170,405</t>
+          <t>KES 162,275</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="13" t="inlineStr">
+      <c r="A24" s="10" t="inlineStr">
         <is>
           <t>TOTAL PROJECT COST:</t>
         </is>
       </c>
-      <c r="B24" s="13" t="inlineStr">
-        <is>
-          <t>KES 1,806,916</t>
+      <c r="B24" s="10" t="inlineStr">
+        <is>
+          <t>KES 1,843,457</t>
         </is>
       </c>
     </row>
@@ -22892,14 +22398,14 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="14" t="inlineStr">
+      <c r="A26" s="11" t="inlineStr">
         <is>
           <t>Additional Funds Needed:</t>
         </is>
       </c>
-      <c r="B26" s="14" t="inlineStr">
-        <is>
-          <t>KES 806,916</t>
+      <c r="B26" s="11" t="inlineStr">
+        <is>
+          <t>KES 843,457</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add tiling labor payment - 14,170 KES
PAYMENT MADE (25/10/2025):
- Tiling labor: 14,170 KES
- Reduces Tile Fixer balance from 30,000 to 15,830 KES

UPDATED TOTALS:
- Total spent: 1,629,508.50 (162.95% of budget)
- Outstanding balances: 51,830 KES (down from 66,000)
  * Electrician: 8,000 KES
  * Plumber: 12,000 KES
  * Painter: 16,000 KES
  * Cabinet Specialist: 0 KES (cleared)
  * Tile Fixer: 15,830 KES (down from 30,000)
- Total pending: 211,979 KES (down from 228,275)
- Additional funds needed: 841,487.50 KES (84.15% over budget)
- Total transactions: 501
</commit_message>
<xml_diff>
--- a/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
+++ b/mum-in-law-house/Mother-In-Law-House-Expenses.xlsx
@@ -535,7 +535,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KES 1,615,182</t>
+          <t>KES 1,629,508</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KES -615,182</t>
+          <t>KES -629,508</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>161.52%</t>
+          <t>162.95%</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KES 18,535</t>
+          <t>KES 18,691</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>KES 66,000</t>
+          <t>KES 51,830</t>
         </is>
       </c>
     </row>
@@ -614,7 +614,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KES 66,000</t>
+          <t>KES 51,830</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KES 1,681,182</t>
+          <t>KES 1,681,338</t>
         </is>
       </c>
     </row>
@@ -638,7 +638,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>168.12%</t>
+          <t>168.13%</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KES -681,182</t>
+          <t>KES -681,338</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KES 162,275</t>
+          <t>KES 160,149</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>KES 1,843,457</t>
+          <t>KES 1,841,487</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>KES 843,457</t>
+          <t>KES 841,487</t>
         </is>
       </c>
     </row>
@@ -759,17 +759,17 @@
         </is>
       </c>
       <c r="B26" s="5" t="n">
-        <v>453935</v>
+        <v>468105</v>
       </c>
       <c r="C26" s="5" t="n">
-        <v>5190.5</v>
+        <v>5346.5</v>
       </c>
       <c r="D26" s="5" t="n">
-        <v>459125.5</v>
+        <v>473451.5</v>
       </c>
       <c r="E26" s="5" t="inlineStr">
         <is>
-          <t>45.91%</t>
+          <t>47.35%</t>
         </is>
       </c>
     </row>
@@ -976,7 +976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I501"/>
+  <dimension ref="A1:I502"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21537,6 +21537,47 @@
         </is>
       </c>
       <c r="I501" s="5" t="inlineStr">
+        <is>
+          <t>PAID</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="5" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="B502" s="5" t="inlineStr">
+        <is>
+          <t>Labor Costs</t>
+        </is>
+      </c>
+      <c r="C502" s="5" t="inlineStr">
+        <is>
+          <t>Specialist Work</t>
+        </is>
+      </c>
+      <c r="D502" s="5" t="inlineStr">
+        <is>
+          <t>Payment for tiling labor</t>
+        </is>
+      </c>
+      <c r="E502" s="5" t="n">
+        <v>14170</v>
+      </c>
+      <c r="F502" s="5" t="n">
+        <v>156</v>
+      </c>
+      <c r="G502" s="5" t="n">
+        <v>14326</v>
+      </c>
+      <c r="H502" s="5" t="inlineStr">
+        <is>
+          <t>Tile Fixer</t>
+        </is>
+      </c>
+      <c r="I502" s="5" t="inlineStr">
         <is>
           <t>PAID</t>
         </is>
@@ -21769,10 +21810,10 @@
         <v>156</v>
       </c>
       <c r="C14" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>1872</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="15">
@@ -21831,7 +21872,7 @@
       </c>
       <c r="B20" s="6" t="inlineStr">
         <is>
-          <t>KES 18,535</t>
+          <t>KES 18,691</t>
         </is>
       </c>
     </row>
@@ -21997,11 +22038,11 @@
       </c>
       <c r="B9" s="5" t="inlineStr">
         <is>
-          <t>Fixing tiles - 30000</t>
+          <t>Fixing tiles - 30000, paid 14170 on 25/10 = 15830 remaining</t>
         </is>
       </c>
       <c r="C9" s="5" t="n">
-        <v>30000</v>
+        <v>15830</v>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
@@ -22017,7 +22058,7 @@
       </c>
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>KES 66,000</t>
+          <t>KES 51,830</t>
         </is>
       </c>
     </row>
@@ -22303,7 +22344,7 @@
         </is>
       </c>
       <c r="C14" s="8" t="n">
-        <v>29775</v>
+        <v>27649</v>
       </c>
     </row>
     <row r="16">
@@ -22314,7 +22355,7 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>KES 162,275</t>
+          <t>KES 160,149</t>
         </is>
       </c>
     </row>
@@ -22333,7 +22374,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KES 1,615,182</t>
+          <t>KES 1,629,508</t>
         </is>
       </c>
     </row>
@@ -22345,7 +22386,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>KES 66,000</t>
+          <t>KES 51,830</t>
         </is>
       </c>
     </row>
@@ -22369,7 +22410,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>KES 162,275</t>
+          <t>KES 160,149</t>
         </is>
       </c>
     </row>
@@ -22381,7 +22422,7 @@
       </c>
       <c r="B24" s="10" t="inlineStr">
         <is>
-          <t>KES 1,843,457</t>
+          <t>KES 1,841,487</t>
         </is>
       </c>
     </row>
@@ -22405,7 +22446,7 @@
       </c>
       <c r="B26" s="11" t="inlineStr">
         <is>
-          <t>KES 843,457</t>
+          <t>KES 841,487</t>
         </is>
       </c>
     </row>

</xml_diff>